<commit_message>
v0.7: updated symbol compatibility
Changes to be committed:
	modified:   prototyping.ipynb
	modified:   qplib/__pycache__/qlang.cpython-313.pyc
	modified:   qplib/data/symbols.csv
	modified:   qplib/data/symbols.xlsx
	modified:   qplib/qlang.py
</commit_message>
<xml_diff>
--- a/qplib/data/symbols.xlsx
+++ b/qplib/data/symbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinVölkl\Desktop\qplib_dev\qplib\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999ABB7D-BD09-43EF-809C-32058B2217CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBE8959-03A0-4E35-90AD-16C739AF07BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-1920" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1430,18 +1430,18 @@
   <dimension ref="A1:CC81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O74" sqref="O74"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.77734375" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
@@ -2526,7 +2526,7 @@
       <c r="CB5" s="2"/>
       <c r="CC5" s="2"/>
     </row>
-    <row r="6" spans="1:81" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>202</v>
       </c>
@@ -2618,7 +2618,7 @@
       <c r="CC6" s="2"/>
     </row>
     <row r="7" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="18" t="s">
         <v>208</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -10545,76 +10545,76 @@
         <v>0</v>
       </c>
       <c r="X60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT60" s="1">
         <v>0</v>
       </c>
       <c r="AU60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV60" s="1">
         <v>0</v>
@@ -10748,76 +10748,76 @@
         <v>0</v>
       </c>
       <c r="X61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT61" s="1">
         <v>0</v>
       </c>
       <c r="AU61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV61" s="1">
         <v>0</v>
@@ -10953,76 +10953,76 @@
         <v>0</v>
       </c>
       <c r="X62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT62" s="1">
         <v>0</v>
       </c>
       <c r="AU62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV62" s="1">
         <v>0</v>
@@ -11160,76 +11160,76 @@
         <v>0</v>
       </c>
       <c r="X63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT63" s="1">
         <v>0</v>
       </c>
       <c r="AU63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV63" s="1">
         <v>0</v>
@@ -11369,76 +11369,76 @@
         <v>0</v>
       </c>
       <c r="X64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT64" s="1">
         <v>0</v>
       </c>
       <c r="AU64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV64" s="1">
         <v>0</v>
@@ -11580,49 +11580,49 @@
         <v>0</v>
       </c>
       <c r="X65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD65" s="1">
         <v>0</v>
       </c>
       <c r="AE65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM65" s="1">
         <v>0</v>
@@ -11649,7 +11649,7 @@
         <v>0</v>
       </c>
       <c r="AU65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV65" s="1">
         <v>0</v>
@@ -11862,7 +11862,7 @@
         <v>0</v>
       </c>
       <c r="AU66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV66" s="1">
         <v>0</v>
@@ -12077,7 +12077,7 @@
         <v>0</v>
       </c>
       <c r="AU67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV67" s="1">
         <v>0</v>
@@ -12294,7 +12294,7 @@
         <v>0</v>
       </c>
       <c r="AU68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV68" s="1">
         <v>0</v>
@@ -12513,7 +12513,7 @@
         <v>0</v>
       </c>
       <c r="AU69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV69" s="1">
         <v>0</v>
@@ -12731,13 +12731,13 @@
         <v>0</v>
       </c>
       <c r="AT70" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU70" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV70" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW70" s="1">
         <v>0</v>
@@ -12954,13 +12954,13 @@
         <v>0</v>
       </c>
       <c r="AT71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW71" s="1">
         <v>0</v>
@@ -13182,7 +13182,7 @@
         <v>0</v>
       </c>
       <c r="AU72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV72" s="1">
         <v>0</v>
@@ -13409,7 +13409,7 @@
         <v>0</v>
       </c>
       <c r="AU73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV73" s="1">
         <v>0</v>
@@ -13638,7 +13638,7 @@
         <v>0</v>
       </c>
       <c r="AU74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV74" s="1">
         <v>0</v>
@@ -13869,7 +13869,7 @@
         <v>0</v>
       </c>
       <c r="AU75" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV75" s="1">
         <v>0</v>
@@ -14102,7 +14102,7 @@
         <v>0</v>
       </c>
       <c r="AU76" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV76" s="1">
         <v>0</v>
@@ -14334,46 +14334,46 @@
         <v>0</v>
       </c>
       <c r="AT77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH77" s="1">
         <v>0</v>
@@ -14571,46 +14571,46 @@
         <v>0</v>
       </c>
       <c r="AT78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW78" s="1">
         <v>0</v>
       </c>
       <c r="AX78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH78" s="1">
         <v>0</v>
@@ -14813,10 +14813,10 @@
         <v>0</v>
       </c>
       <c r="AU79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW79" s="1">
         <v>0</v>
@@ -15054,10 +15054,10 @@
         <v>0</v>
       </c>
       <c r="AU80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW80" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
published v0.7.0 changes: - symbols are now defined in symbols.csv - symbols.csv includes compatibility information - more extensive validation of instructions - tests now also check correct logging - df.qi() currently disabled
Changes to be committed:
	deleted:    dist/qplib-0.6.2-py3-none-any.whl
	deleted:    dist/qplib-0.6.2.tar.gz
	new file:   dist/qplib-0.7.0-py3-none-any.whl
	new file:   dist/qplib-0.7.0.tar.gz
	modified:   pyproject.toml
	modified:   qplib.egg-info/PKG-INFO
	modified:   qplib.egg-info/SOURCES.txt
	modified:   qplib/__pycache__/qlang.cpython-313.pyc
	modified:   qplib/__pycache__/util.cpython-313.pyc
	modified:   qplib/data/symbols.csv
	modified:   qplib/data/symbols.xlsx
	modified:   qplib/qlang.py
	deleted:    qplib/qlang_old.py
</commit_message>
<xml_diff>
--- a/qplib/data/symbols.xlsx
+++ b/qplib/data/symbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinVölkl\Desktop\qplib_dev\qplib\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBE8959-03A0-4E35-90AD-16C739AF07BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5269DCE1-8322-48D7-A692-9B7B8CB613B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-1920" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -705,7 +705,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,12 +719,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1430,10 +1424,10 @@
   <dimension ref="A1:CC81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="BG70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomRight" activeCell="BL71" sqref="BL71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6357,7 +6351,7 @@
       <c r="CB36" s="1"/>
       <c r="CC36" s="1"/>
     </row>
-    <row r="37" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
         <v>88</v>
       </c>
@@ -6997,7 +6991,7 @@
       <c r="CB40" s="1"/>
       <c r="CC40" s="1"/>
     </row>
-    <row r="41" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
         <v>92</v>
       </c>
@@ -7329,7 +7323,7 @@
       <c r="CB42" s="1"/>
       <c r="CC42" s="1"/>
     </row>
-    <row r="43" spans="1:81" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
         <v>94</v>
       </c>
@@ -7498,7 +7492,7 @@
       <c r="CB43" s="1"/>
       <c r="CC43" s="1"/>
     </row>
-    <row r="44" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
         <v>95</v>
       </c>
@@ -7669,7 +7663,7 @@
       <c r="CB44" s="1"/>
       <c r="CC44" s="1"/>
     </row>
-    <row r="45" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
         <v>96</v>
       </c>
@@ -8554,7 +8548,7 @@
       <c r="CB49" s="1"/>
       <c r="CC49" s="1"/>
     </row>
-    <row r="50" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A50" s="31" t="s">
         <v>99</v>
       </c>
@@ -8737,7 +8731,7 @@
       <c r="CB50" s="1"/>
       <c r="CC50" s="1"/>
     </row>
-    <row r="51" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
         <v>100</v>
       </c>
@@ -8922,7 +8916,7 @@
       <c r="CB51" s="1"/>
       <c r="CC51" s="1"/>
     </row>
-    <row r="52" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A52" s="31" t="s">
         <v>101</v>
       </c>
@@ -9109,7 +9103,7 @@
       <c r="CB52" s="1"/>
       <c r="CC52" s="1"/>
     </row>
-    <row r="53" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
         <v>102</v>
       </c>
@@ -9298,7 +9292,7 @@
       <c r="CB53" s="1"/>
       <c r="CC53" s="1"/>
     </row>
-    <row r="54" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
         <v>103</v>
       </c>
@@ -9489,7 +9483,7 @@
       <c r="CB54" s="1"/>
       <c r="CC54" s="1"/>
     </row>
-    <row r="55" spans="1:81" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="31" t="s">
         <v>104</v>
       </c>
@@ -9682,7 +9676,7 @@
       <c r="CB55" s="1"/>
       <c r="CC55" s="1"/>
     </row>
-    <row r="56" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A56" s="31" t="s">
         <v>105</v>
       </c>
@@ -10617,7 +10611,7 @@
         <v>1</v>
       </c>
       <c r="AV60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW60" s="1">
         <v>0</v>
@@ -10820,7 +10814,7 @@
         <v>1</v>
       </c>
       <c r="AV61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW61" s="1">
         <v>0</v>
@@ -10856,7 +10850,7 @@
         <v>0</v>
       </c>
       <c r="BH61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI61" s="1">
         <v>3</v>
@@ -11025,7 +11019,7 @@
         <v>1</v>
       </c>
       <c r="AV62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW62" s="1">
         <v>0</v>
@@ -11061,7 +11055,7 @@
         <v>0</v>
       </c>
       <c r="BH62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI62" s="1">
         <v>0</v>
@@ -11232,7 +11226,7 @@
         <v>1</v>
       </c>
       <c r="AV63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW63" s="1">
         <v>0</v>
@@ -11268,7 +11262,7 @@
         <v>0</v>
       </c>
       <c r="BH63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI63" s="1">
         <v>0</v>
@@ -11441,7 +11435,7 @@
         <v>1</v>
       </c>
       <c r="AV64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW64" s="1">
         <v>0</v>
@@ -11477,7 +11471,7 @@
         <v>0</v>
       </c>
       <c r="BH64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI64" s="1">
         <v>0</v>
@@ -11509,7 +11503,7 @@
       <c r="CB64" s="1"/>
       <c r="CC64" s="1"/>
     </row>
-    <row r="65" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:81" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="33" t="s">
         <v>116</v>
       </c>
@@ -11688,19 +11682,19 @@
         <v>0</v>
       </c>
       <c r="BH65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM65" s="1">
         <v>3</v>
@@ -12154,7 +12148,7 @@
       <c r="CB67" s="1"/>
       <c r="CC67" s="1"/>
     </row>
-    <row r="68" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:81" x14ac:dyDescent="0.3">
       <c r="A68" s="33" t="s">
         <v>119</v>
       </c>
@@ -13042,7 +13036,7 @@
       <c r="CB71" s="1"/>
       <c r="CC71" s="1"/>
     </row>
-    <row r="72" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="33" t="s">
         <v>123</v>
       </c>
@@ -13729,7 +13723,7 @@
       <c r="CB74" s="1"/>
       <c r="CC74" s="1"/>
     </row>
-    <row r="75" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="33" t="s">
         <v>126</v>
       </c>
@@ -15096,16 +15090,16 @@
         <v>0</v>
       </c>
       <c r="BI80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM80" s="1">
         <v>0</v>
@@ -15123,7 +15117,7 @@
         <v>0</v>
       </c>
       <c r="BR80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS80" s="1">
         <v>0</v>
@@ -15240,10 +15234,10 @@
         <v>0</v>
       </c>
       <c r="AB81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD81" s="1">
         <v>0</v>
@@ -15336,10 +15330,10 @@
         <v>0</v>
       </c>
       <c r="BH81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ81" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
cleanup and minor fixes
Changes to be committed:
	modified:   interactive_demo.ipynb
	modified:   prototyping.ipynb
	modified:   qplib/__pycache__/qlang.cpython-313.pyc
	modified:   qplib/data/symbols.csv
	modified:   qplib/data/symbols.xlsx
	modified:   qplib/qlang.py
	modified:   tests/__pycache__/test_qlang.cpython-313-pytest-8.3.4.pyc
	modified:   tests/test_qlang.py
</commit_message>
<xml_diff>
--- a/qplib/data/symbols.xlsx
+++ b/qplib/data/symbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinVölkl\Desktop\qplib_dev\qplib\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5269DCE1-8322-48D7-A692-9B7B8CB613B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AE9F3A-CC82-48FC-97D5-3A6B78C3377E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-1920" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1424,10 +1424,10 @@
   <dimension ref="A1:CC81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="BG70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="BE57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BL71" sqref="BL71"/>
+      <selection pane="bottomRight" activeCell="BJ67" sqref="BJ67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11595,7 +11595,7 @@
         <v>0</v>
       </c>
       <c r="AE65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF65" s="1">
         <v>1</v>
@@ -11610,10 +11610,10 @@
         <v>1</v>
       </c>
       <c r="AJ65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL65" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
added and tested TRIM operator
Changes to be committed:
	modified:   qplib/__pycache__/qlang.cpython-313.pyc
	modified:   qplib/data/symbols.csv
	modified:   qplib/data/symbols.xlsx
	modified:   qplib/qlang.py
	modified:   tests/__pycache__/test_qlang.cpython-313-pytest-8.3.4.pyc
	modified:   tests/test_qlang.py
</commit_message>
<xml_diff>
--- a/qplib/data/symbols.xlsx
+++ b/qplib/data/symbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinVölkl\Desktop\qplib_dev\qplib\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AE9F3A-CC82-48FC-97D5-3A6B78C3377E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A84B1A-EB19-4F33-BEB3-792AC86CBE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-1920" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$CC$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$CD$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="217">
   <si>
     <t>"%%"</t>
   </si>
@@ -699,6 +699,15 @@
   </si>
   <si>
     <t>is_type</t>
+  </si>
+  <si>
+    <t>TRIM</t>
+  </si>
+  <si>
+    <t>"trim;"</t>
+  </si>
+  <si>
+    <t>trim all cols where no row values were selected</t>
   </si>
 </sst>
 </file>
@@ -1421,13 +1430,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC81"/>
+  <dimension ref="A1:CD82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="BE57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="W21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BJ67" sqref="BJ67"/>
+      <selection pane="bottomRight" activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,60 +1465,61 @@
     <col min="27" max="27" width="11.77734375" style="38" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12.44140625" style="38" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="27.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="27.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.44140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16" style="38" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.44140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.44140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.44140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="23.21875" style="38" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="29.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="28.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="27.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="20" style="38" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="30.44140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="30" style="38" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="29.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14" style="38" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="29.44140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="26.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="21" style="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="18.77734375" style="38" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="21.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="21.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="22.77734375" style="38" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="18.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="26.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="29.44140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="27.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="29.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="30.21875" style="38" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="29.44140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="28.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="30.44140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="29" style="38" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="30.77734375" style="38" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="29" style="38" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="30.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="29.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="30.77734375" style="38" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="25.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="30.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="30.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="26.21875" style="38" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="30.21875" style="38" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="25.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="28.21875" style="38" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="30" style="38" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="28.5546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="28.21875" style="38" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="27.88671875" style="38" customWidth="1"/>
+    <col min="31" max="31" width="27.109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16" style="38" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23.21875" style="38" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="29.109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="27.88671875" style="38" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="20" style="38" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="30.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="30" style="38" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="29.88671875" style="38" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14" style="38" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="29.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="26.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="21" style="38" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.77734375" style="38" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="21.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.88671875" style="38" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="22.77734375" style="38" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="18.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="26.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="29.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="27.88671875" style="38" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="29.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="62" max="63" width="30.21875" style="38" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="29.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="28.88671875" style="38" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="30.44140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="29" style="38" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="30.77734375" style="38" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="29" style="38" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="30.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="29.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="30.77734375" style="38" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="25.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="30.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="30.109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="26.21875" style="38" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="30.21875" style="38" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="25.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="28.21875" style="38" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="30" style="38" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="28.5546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="28.21875" style="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:82" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>198</v>
@@ -1596,163 +1606,166 @@
         <v>80</v>
       </c>
       <c r="AD1" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" s="15" t="s">
+      <c r="AF1" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" s="15" t="s">
+      <c r="AG1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AI1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AJ1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AK1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="AK1" s="15" t="s">
+      <c r="AL1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AL1" s="15" t="s">
+      <c r="AM1" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="AM1" s="15" t="s">
+      <c r="AN1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="AN1" s="15" t="s">
+      <c r="AO1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="AO1" s="15" t="s">
+      <c r="AP1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="AP1" s="15" t="s">
+      <c r="AQ1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="AQ1" s="15" t="s">
+      <c r="AR1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="AR1" s="15" t="s">
+      <c r="AS1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="AS1" s="15" t="s">
+      <c r="AT1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="AT1" s="15" t="s">
+      <c r="AU1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="AU1" s="15" t="s">
+      <c r="AV1" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="AV1" s="15" t="s">
+      <c r="AW1" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="AW1" s="15" t="s">
+      <c r="AX1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="AX1" s="15" t="s">
+      <c r="AY1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="AY1" s="15" t="s">
+      <c r="AZ1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="AZ1" s="15" t="s">
+      <c r="BA1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="BA1" s="15" t="s">
+      <c r="BB1" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="BB1" s="15" t="s">
+      <c r="BC1" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="BC1" s="15" t="s">
+      <c r="BD1" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="BD1" s="15" t="s">
+      <c r="BE1" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="BE1" s="15" t="s">
+      <c r="BF1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="BF1" s="15" t="s">
+      <c r="BG1" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="BG1" s="15" t="s">
+      <c r="BH1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="BH1" s="16" t="s">
+      <c r="BI1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="BI1" s="16" t="s">
+      <c r="BJ1" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="BJ1" s="16" t="s">
+      <c r="BK1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="BK1" s="16" t="s">
+      <c r="BL1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="BL1" s="16" t="s">
+      <c r="BM1" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="BM1" s="16" t="s">
+      <c r="BN1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="BN1" s="16" t="s">
+      <c r="BO1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="BO1" s="16" t="s">
+      <c r="BP1" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="BP1" s="16" t="s">
+      <c r="BQ1" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="BQ1" s="16" t="s">
+      <c r="BR1" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="BR1" s="16" t="s">
+      <c r="BS1" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="BS1" s="16" t="s">
+      <c r="BT1" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="BT1" s="16" t="s">
+      <c r="BU1" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="BU1" s="16" t="s">
+      <c r="BV1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="BV1" s="16" t="s">
+      <c r="BW1" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="BW1" s="16" t="s">
+      <c r="BX1" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="BX1" s="16" t="s">
+      <c r="BY1" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="BY1" s="16" t="s">
+      <c r="BZ1" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="BZ1" s="16" t="s">
+      <c r="CA1" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="CA1" s="16" t="s">
+      <c r="CB1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="CB1" s="16" t="s">
+      <c r="CC1" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="CC1" s="16" t="s">
+      <c r="CD1" s="16" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:81" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:82" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>198</v>
       </c>
@@ -1930,8 +1943,8 @@
       <c r="BG2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BH2" s="5" t="s">
-        <v>67</v>
+      <c r="BH2" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="BI2" s="5" t="s">
         <v>67</v>
@@ -1996,8 +2009,11 @@
       <c r="CC2" s="5" t="s">
         <v>67</v>
       </c>
+      <c r="CD2" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="3" spans="1:81" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:82" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>204</v>
       </c>
@@ -2058,163 +2074,166 @@
         <v>12</v>
       </c>
       <c r="AD3" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AE3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AE3" s="4" t="s">
+      <c r="AF3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AF3" s="4" t="s">
+      <c r="AG3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AH3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AK3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AK3" s="4" t="s">
+      <c r="AL3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AM3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AM3" s="4" t="s">
+      <c r="AN3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AN3" s="4" t="s">
+      <c r="AO3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AO3" s="4" t="s">
+      <c r="AP3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AP3" s="4" t="s">
+      <c r="AQ3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AQ3" s="4" t="s">
+      <c r="AR3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AR3" s="4" t="s">
+      <c r="AS3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AS3" s="4" t="s">
+      <c r="AT3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AT3" s="4" t="s">
+      <c r="AU3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AU3" s="4" t="s">
+      <c r="AV3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AV3" s="4" t="s">
+      <c r="AW3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AW3" s="4" t="s">
+      <c r="AX3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AX3" s="4" t="s">
+      <c r="AY3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AY3" s="4" t="s">
+      <c r="AZ3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AZ3" s="4" t="s">
+      <c r="BA3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="BA3" s="4" t="s">
+      <c r="BB3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="BB3" s="4" t="s">
+      <c r="BC3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="BC3" s="4" t="s">
+      <c r="BD3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="BD3" s="4" t="s">
+      <c r="BE3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BE3" s="4" t="s">
+      <c r="BF3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="BF3" s="4" t="s">
+      <c r="BG3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BG3" s="4" t="s">
+      <c r="BH3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="BH3" s="5" t="s">
+      <c r="BI3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="BI3" s="5" t="s">
+      <c r="BJ3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="BJ3" s="5" t="s">
+      <c r="BK3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BK3" s="5" t="s">
+      <c r="BL3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="BL3" s="5" t="s">
+      <c r="BM3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="BM3" s="5" t="s">
+      <c r="BN3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="BN3" s="5" t="s">
+      <c r="BO3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="BO3" s="5" t="s">
+      <c r="BP3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="BP3" s="5" t="s">
+      <c r="BQ3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="BQ3" s="5" t="s">
+      <c r="BR3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="BR3" s="5" t="s">
+      <c r="BS3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="BS3" s="5" t="s">
+      <c r="BT3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="BT3" s="5" t="s">
+      <c r="BU3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="BU3" s="5" t="s">
+      <c r="BV3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="BV3" s="5" t="s">
+      <c r="BW3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="BW3" s="5" t="s">
+      <c r="BX3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="BX3" s="5" t="s">
+      <c r="BY3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="BY3" s="5" t="s">
+      <c r="BZ3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="BZ3" s="5" t="s">
+      <c r="CA3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="CA3" s="5" t="s">
+      <c r="CB3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="CB3" s="5" t="s">
+      <c r="CC3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="CC3" s="5" t="s">
+      <c r="CD3" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:81" s="23" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:82" s="23" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>199</v>
       </c>
@@ -2275,163 +2294,166 @@
         <v>145</v>
       </c>
       <c r="AD4" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="AE4" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="AE4" s="21" t="s">
+      <c r="AF4" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="AF4" s="21" t="s">
+      <c r="AG4" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="AG4" s="21" t="s">
+      <c r="AH4" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="AH4" s="21" t="s">
+      <c r="AI4" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="AI4" s="21" t="s">
+      <c r="AJ4" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="AJ4" s="21" t="s">
+      <c r="AK4" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="AK4" s="21" t="s">
+      <c r="AL4" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="AL4" s="21" t="s">
+      <c r="AM4" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="AM4" s="21" t="s">
+      <c r="AN4" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="AN4" s="21" t="s">
+      <c r="AO4" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="AO4" s="21" t="s">
+      <c r="AP4" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="AP4" s="21" t="s">
+      <c r="AQ4" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="AQ4" s="21" t="s">
+      <c r="AR4" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="AR4" s="21" t="s">
+      <c r="AS4" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="AS4" s="21" t="s">
+      <c r="AT4" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="AT4" s="21" t="s">
+      <c r="AU4" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="AU4" s="21" t="s">
+      <c r="AV4" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="AV4" s="21" t="s">
+      <c r="AW4" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="AW4" s="21" t="s">
+      <c r="AX4" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="AX4" s="21" t="s">
+      <c r="AY4" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="AY4" s="21" t="s">
+      <c r="AZ4" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="AZ4" s="21" t="s">
+      <c r="BA4" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="BA4" s="21" t="s">
+      <c r="BB4" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="BB4" s="21" t="s">
+      <c r="BC4" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="BC4" s="21" t="s">
+      <c r="BD4" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="BD4" s="21" t="s">
+      <c r="BE4" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="BE4" s="21" t="s">
+      <c r="BF4" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="BF4" s="21" t="s">
+      <c r="BG4" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="BG4" s="21" t="s">
+      <c r="BH4" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="BH4" s="22" t="s">
+      <c r="BI4" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="BI4" s="22" t="s">
+      <c r="BJ4" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="BJ4" s="22" t="s">
+      <c r="BK4" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="BK4" s="22" t="s">
+      <c r="BL4" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="BL4" s="22" t="s">
+      <c r="BM4" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="BM4" s="22" t="s">
+      <c r="BN4" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="BN4" s="22" t="s">
+      <c r="BO4" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="BO4" s="22" t="s">
+      <c r="BP4" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="BP4" s="22" t="s">
+      <c r="BQ4" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="BQ4" s="22" t="s">
+      <c r="BR4" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="BR4" s="22" t="s">
+      <c r="BS4" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="BS4" s="22" t="s">
+      <c r="BT4" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="BT4" s="22" t="s">
+      <c r="BU4" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="BU4" s="22" t="s">
+      <c r="BV4" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="BV4" s="22" t="s">
+      <c r="BW4" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="BW4" s="22" t="s">
+      <c r="BX4" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="BX4" s="22" t="s">
+      <c r="BY4" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="BY4" s="22" t="s">
+      <c r="BZ4" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="BZ4" s="22" t="s">
+      <c r="CA4" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="CA4" s="22" t="s">
+      <c r="CB4" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="CB4" s="22" t="s">
+      <c r="CC4" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="CC4" s="22" t="s">
+      <c r="CD4" s="22" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>201</v>
       </c>
@@ -2519,8 +2541,9 @@
       <c r="CA5" s="2"/>
       <c r="CB5" s="2"/>
       <c r="CC5" s="2"/>
+      <c r="CD5" s="2"/>
     </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>202</v>
       </c>
@@ -2610,8 +2633,9 @@
       <c r="CA6" s="2"/>
       <c r="CB6" s="2"/>
       <c r="CC6" s="2"/>
+      <c r="CD6" s="2"/>
     </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>208</v>
       </c>
@@ -2703,8 +2727,9 @@
       <c r="CA7" s="2"/>
       <c r="CB7" s="2"/>
       <c r="CC7" s="2"/>
+      <c r="CD7" s="2"/>
     </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>203</v>
       </c>
@@ -2798,8 +2823,9 @@
       <c r="CA8" s="2"/>
       <c r="CB8" s="2"/>
       <c r="CC8" s="2"/>
+      <c r="CD8" s="2"/>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>207</v>
       </c>
@@ -2895,8 +2921,9 @@
       <c r="CA9" s="2"/>
       <c r="CB9" s="2"/>
       <c r="CC9" s="2"/>
+      <c r="CD9" s="2"/>
     </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>200</v>
       </c>
@@ -2994,8 +3021,9 @@
       <c r="CA10" s="2"/>
       <c r="CB10" s="2"/>
       <c r="CC10" s="2"/>
+      <c r="CD10" s="2"/>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>205</v>
       </c>
@@ -3095,8 +3123,9 @@
       <c r="CA11" s="2"/>
       <c r="CB11" s="2"/>
       <c r="CC11" s="2"/>
+      <c r="CD11" s="2"/>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>209</v>
       </c>
@@ -3198,8 +3227,9 @@
       <c r="CA12" s="2"/>
       <c r="CB12" s="2"/>
       <c r="CC12" s="2"/>
+      <c r="CD12" s="2"/>
     </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>210</v>
       </c>
@@ -3303,8 +3333,9 @@
       <c r="CA13" s="2"/>
       <c r="CB13" s="2"/>
       <c r="CC13" s="2"/>
+      <c r="CD13" s="2"/>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>211</v>
       </c>
@@ -3410,8 +3441,9 @@
       <c r="CA14" s="2"/>
       <c r="CB14" s="2"/>
       <c r="CC14" s="2"/>
+      <c r="CD14" s="2"/>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>212</v>
       </c>
@@ -3519,8 +3551,9 @@
       <c r="CA15" s="2"/>
       <c r="CB15" s="2"/>
       <c r="CC15" s="2"/>
+      <c r="CD15" s="2"/>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>213</v>
       </c>
@@ -3630,8 +3663,9 @@
       <c r="CA16" s="2"/>
       <c r="CB16" s="2"/>
       <c r="CC16" s="2"/>
+      <c r="CD16" s="2"/>
     </row>
-    <row r="17" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>68</v>
       </c>
@@ -3747,8 +3781,9 @@
       <c r="CA17" s="1"/>
       <c r="CB17" s="1"/>
       <c r="CC17" s="1"/>
+      <c r="CD17" s="1"/>
     </row>
-    <row r="18" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>69</v>
       </c>
@@ -3866,8 +3901,9 @@
       <c r="CA18" s="1"/>
       <c r="CB18" s="1"/>
       <c r="CC18" s="1"/>
+      <c r="CD18" s="1"/>
     </row>
-    <row r="19" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>70</v>
       </c>
@@ -3987,8 +4023,9 @@
       <c r="CA19" s="1"/>
       <c r="CB19" s="1"/>
       <c r="CC19" s="1"/>
+      <c r="CD19" s="1"/>
     </row>
-    <row r="20" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>71</v>
       </c>
@@ -4110,8 +4147,9 @@
       <c r="CA20" s="1"/>
       <c r="CB20" s="1"/>
       <c r="CC20" s="1"/>
+      <c r="CD20" s="1"/>
     </row>
-    <row r="21" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:82" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>72</v>
       </c>
@@ -4235,8 +4273,9 @@
       <c r="CA21" s="1"/>
       <c r="CB21" s="1"/>
       <c r="CC21" s="1"/>
+      <c r="CD21" s="1"/>
     </row>
-    <row r="22" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:82" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
         <v>73</v>
       </c>
@@ -4362,8 +4401,9 @@
       <c r="CA22" s="1"/>
       <c r="CB22" s="1"/>
       <c r="CC22" s="1"/>
+      <c r="CD22" s="1"/>
     </row>
-    <row r="23" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:82" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
         <v>74</v>
       </c>
@@ -4491,8 +4531,9 @@
       <c r="CA23" s="1"/>
       <c r="CB23" s="1"/>
       <c r="CC23" s="1"/>
+      <c r="CD23" s="1"/>
     </row>
-    <row r="24" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A24" s="31" t="s">
         <v>75</v>
       </c>
@@ -4622,8 +4663,9 @@
       <c r="CA24" s="1"/>
       <c r="CB24" s="1"/>
       <c r="CC24" s="1"/>
+      <c r="CD24" s="1"/>
     </row>
-    <row r="25" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
         <v>76</v>
       </c>
@@ -4755,8 +4797,9 @@
       <c r="CA25" s="1"/>
       <c r="CB25" s="1"/>
       <c r="CC25" s="1"/>
+      <c r="CD25" s="1"/>
     </row>
-    <row r="26" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
         <v>77</v>
       </c>
@@ -4890,8 +4933,9 @@
       <c r="CA26" s="1"/>
       <c r="CB26" s="1"/>
       <c r="CC26" s="1"/>
+      <c r="CD26" s="1"/>
     </row>
-    <row r="27" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>78</v>
       </c>
@@ -5027,8 +5071,9 @@
       <c r="CA27" s="1"/>
       <c r="CB27" s="1"/>
       <c r="CC27" s="1"/>
+      <c r="CD27" s="1"/>
     </row>
-    <row r="28" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A28" s="31" t="s">
         <v>79</v>
       </c>
@@ -5166,8 +5211,9 @@
       <c r="CA28" s="1"/>
       <c r="CB28" s="1"/>
       <c r="CC28" s="1"/>
+      <c r="CD28" s="1"/>
     </row>
-    <row r="29" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="31" t="s">
         <v>80</v>
       </c>
@@ -5307,28 +5353,29 @@
       <c r="CA29" s="1"/>
       <c r="CB29" s="1"/>
       <c r="CC29" s="1"/>
+      <c r="CD29" s="1"/>
     </row>
-    <row r="30" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="31" t="s">
-        <v>81</v>
+    <row r="30" spans="1:82" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
+        <v>214</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>146</v>
+        <v>215</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>216</v>
       </c>
       <c r="E30" s="2">
         <v>2</v>
       </c>
       <c r="F30" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="2">
         <v>2</v>
@@ -5358,13 +5405,13 @@
         <v>0</v>
       </c>
       <c r="Q30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T30" s="1">
         <v>1</v>
@@ -5450,19 +5497,20 @@
       <c r="CA30" s="1"/>
       <c r="CB30" s="1"/>
       <c r="CC30" s="1"/>
+      <c r="CD30" s="1"/>
     </row>
-    <row r="31" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E31" s="2">
         <v>2</v>
@@ -5498,7 +5546,7 @@
         <v>0</v>
       </c>
       <c r="P31" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="1">
         <v>1</v>
@@ -5595,19 +5643,20 @@
       <c r="CA31" s="1"/>
       <c r="CB31" s="1"/>
       <c r="CC31" s="1"/>
+      <c r="CD31" s="1"/>
     </row>
-    <row r="32" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A32" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E32" s="2">
         <v>2</v>
@@ -5742,19 +5791,20 @@
       <c r="CA32" s="1"/>
       <c r="CB32" s="1"/>
       <c r="CC32" s="1"/>
+      <c r="CD32" s="1"/>
     </row>
-    <row r="33" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E33" s="2">
         <v>2</v>
@@ -5891,19 +5941,20 @@
       <c r="CA33" s="1"/>
       <c r="CB33" s="1"/>
       <c r="CC33" s="1"/>
+      <c r="CD33" s="1"/>
     </row>
-    <row r="34" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A34" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E34" s="2">
         <v>2</v>
@@ -6042,19 +6093,20 @@
       <c r="CA34" s="1"/>
       <c r="CB34" s="1"/>
       <c r="CC34" s="1"/>
+      <c r="CD34" s="1"/>
     </row>
-    <row r="35" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E35" s="2">
         <v>2</v>
@@ -6195,19 +6247,20 @@
       <c r="CA35" s="1"/>
       <c r="CB35" s="1"/>
       <c r="CC35" s="1"/>
+      <c r="CD35" s="1"/>
     </row>
-    <row r="36" spans="1:81" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E36" s="2">
         <v>2</v>
@@ -6350,19 +6403,20 @@
       <c r="CA36" s="1"/>
       <c r="CB36" s="1"/>
       <c r="CC36" s="1"/>
+      <c r="CD36" s="1"/>
     </row>
-    <row r="37" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E37" s="2">
         <v>2</v>
@@ -6507,19 +6561,20 @@
       <c r="CA37" s="1"/>
       <c r="CB37" s="1"/>
       <c r="CC37" s="1"/>
+      <c r="CD37" s="1"/>
     </row>
-    <row r="38" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E38" s="2">
         <v>2</v>
@@ -6666,19 +6721,20 @@
       <c r="CA38" s="1"/>
       <c r="CB38" s="1"/>
       <c r="CC38" s="1"/>
+      <c r="CD38" s="1"/>
     </row>
-    <row r="39" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E39" s="2">
         <v>2</v>
@@ -6714,7 +6770,7 @@
         <v>0</v>
       </c>
       <c r="P39" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q39" s="1">
         <v>1</v>
@@ -6827,19 +6883,20 @@
       <c r="CA39" s="1"/>
       <c r="CB39" s="1"/>
       <c r="CC39" s="1"/>
+      <c r="CD39" s="1"/>
     </row>
-    <row r="40" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A40" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E40" s="2">
         <v>2</v>
@@ -6990,19 +7047,20 @@
       <c r="CA40" s="1"/>
       <c r="CB40" s="1"/>
       <c r="CC40" s="1"/>
+      <c r="CD40" s="1"/>
     </row>
-    <row r="41" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E41" s="2">
         <v>2</v>
@@ -7155,19 +7213,20 @@
       <c r="CA41" s="1"/>
       <c r="CB41" s="1"/>
       <c r="CC41" s="1"/>
+      <c r="CD41" s="1"/>
     </row>
-    <row r="42" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E42" s="2">
         <v>2</v>
@@ -7322,19 +7381,20 @@
       <c r="CA42" s="1"/>
       <c r="CB42" s="1"/>
       <c r="CC42" s="1"/>
+      <c r="CD42" s="1"/>
     </row>
-    <row r="43" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E43" s="2">
         <v>2</v>
@@ -7491,19 +7551,20 @@
       <c r="CA43" s="1"/>
       <c r="CB43" s="1"/>
       <c r="CC43" s="1"/>
+      <c r="CD43" s="1"/>
     </row>
-    <row r="44" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E44" s="2">
         <v>2</v>
@@ -7662,19 +7723,20 @@
       <c r="CA44" s="1"/>
       <c r="CB44" s="1"/>
       <c r="CC44" s="1"/>
+      <c r="CD44" s="1"/>
     </row>
-    <row r="45" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E45" s="2">
         <v>2</v>
@@ -7835,37 +7897,38 @@
       <c r="CA45" s="1"/>
       <c r="CB45" s="1"/>
       <c r="CC45" s="1"/>
+      <c r="CD45" s="1"/>
     </row>
-    <row r="46" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A46" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E46" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F46" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I46" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J46" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K46" s="2">
         <v>0</v>
@@ -7880,31 +7943,31 @@
         <v>0</v>
       </c>
       <c r="O46" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P46" s="2">
         <v>0</v>
       </c>
       <c r="Q46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X46" s="1">
         <v>0</v>
@@ -8010,19 +8073,20 @@
       <c r="CA46" s="1"/>
       <c r="CB46" s="1"/>
       <c r="CC46" s="1"/>
+      <c r="CD46" s="1"/>
     </row>
-    <row r="47" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="31" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E47" s="2">
         <v>0</v>
@@ -8046,10 +8110,10 @@
         <v>0</v>
       </c>
       <c r="L47" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M47" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N47" s="2">
         <v>0</v>
@@ -8061,22 +8125,22 @@
         <v>0</v>
       </c>
       <c r="Q47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W47" s="1">
         <v>1</v>
@@ -8187,31 +8251,32 @@
       <c r="CA47" s="1"/>
       <c r="CB47" s="1"/>
       <c r="CC47" s="1"/>
+      <c r="CD47" s="1"/>
     </row>
-    <row r="48" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E48" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F48" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I48" s="2">
         <v>2</v>
@@ -8223,10 +8288,10 @@
         <v>0</v>
       </c>
       <c r="L48" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M48" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N48" s="2">
         <v>0</v>
@@ -8366,37 +8431,38 @@
       <c r="CA48" s="1"/>
       <c r="CB48" s="1"/>
       <c r="CC48" s="1"/>
+      <c r="CD48" s="1"/>
     </row>
-    <row r="49" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="E49" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F49" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I49" s="2">
         <v>2</v>
       </c>
       <c r="J49" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K49" s="2">
         <v>0</v>
@@ -8417,22 +8483,22 @@
         <v>0</v>
       </c>
       <c r="Q49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W49" s="1">
         <v>1</v>
@@ -8547,19 +8613,20 @@
       <c r="CA49" s="1"/>
       <c r="CB49" s="1"/>
       <c r="CC49" s="1"/>
+      <c r="CD49" s="1"/>
     </row>
-    <row r="50" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E50" s="2">
         <v>0</v>
@@ -8580,7 +8647,7 @@
         <v>2</v>
       </c>
       <c r="K50" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L50" s="2">
         <v>0</v>
@@ -8730,19 +8797,20 @@
       <c r="CA50" s="1"/>
       <c r="CB50" s="1"/>
       <c r="CC50" s="1"/>
+      <c r="CD50" s="1"/>
     </row>
-    <row r="51" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E51" s="2">
         <v>0</v>
@@ -8915,19 +8983,20 @@
       <c r="CA51" s="1"/>
       <c r="CB51" s="1"/>
       <c r="CC51" s="1"/>
+      <c r="CD51" s="1"/>
     </row>
-    <row r="52" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A52" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E52" s="2">
         <v>0</v>
@@ -9102,19 +9171,20 @@
       <c r="CA52" s="1"/>
       <c r="CB52" s="1"/>
       <c r="CC52" s="1"/>
+      <c r="CD52" s="1"/>
     </row>
-    <row r="53" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E53" s="2">
         <v>0</v>
@@ -9291,19 +9361,20 @@
       <c r="CA53" s="1"/>
       <c r="CB53" s="1"/>
       <c r="CC53" s="1"/>
+      <c r="CD53" s="1"/>
     </row>
-    <row r="54" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E54" s="2">
         <v>0</v>
@@ -9482,19 +9553,20 @@
       <c r="CA54" s="1"/>
       <c r="CB54" s="1"/>
       <c r="CC54" s="1"/>
+      <c r="CD54" s="1"/>
     </row>
-    <row r="55" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A55" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E55" s="2">
         <v>0</v>
@@ -9675,19 +9747,20 @@
       <c r="CA55" s="1"/>
       <c r="CB55" s="1"/>
       <c r="CC55" s="1"/>
+      <c r="CD55" s="1"/>
     </row>
-    <row r="56" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E56" s="2">
         <v>0</v>
@@ -9870,19 +9943,20 @@
       <c r="CA56" s="1"/>
       <c r="CB56" s="1"/>
       <c r="CC56" s="1"/>
+      <c r="CD56" s="1"/>
     </row>
-    <row r="57" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A57" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E57" s="2">
         <v>0</v>
@@ -10067,19 +10141,20 @@
       <c r="CA57" s="1"/>
       <c r="CB57" s="1"/>
       <c r="CC57" s="1"/>
+      <c r="CD57" s="1"/>
     </row>
-    <row r="58" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A58" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E58" s="2">
         <v>0</v>
@@ -10266,19 +10341,20 @@
       <c r="CA58" s="1"/>
       <c r="CB58" s="1"/>
       <c r="CC58" s="1"/>
+      <c r="CD58" s="1"/>
     </row>
-    <row r="59" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A59" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
@@ -10467,40 +10543,41 @@
       <c r="CA59" s="1"/>
       <c r="CB59" s="1"/>
       <c r="CC59" s="1"/>
+      <c r="CD59" s="1"/>
     </row>
-    <row r="60" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="A60" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D60" s="34" t="s">
-        <v>180</v>
+    <row r="60" spans="1:82" x14ac:dyDescent="0.3">
+      <c r="A60" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>173</v>
       </c>
       <c r="E60" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F60" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I60" s="2">
-        <v>0</v>
-      </c>
-      <c r="J60" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J60" s="2">
+        <v>2</v>
       </c>
       <c r="K60" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L60" s="2">
         <v>0</v>
@@ -10512,106 +10589,106 @@
         <v>0</v>
       </c>
       <c r="O60" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P60" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT60" s="1">
         <v>0</v>
       </c>
       <c r="AU60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW60" s="1">
         <v>0</v>
@@ -10670,19 +10747,20 @@
       <c r="CA60" s="1"/>
       <c r="CB60" s="1"/>
       <c r="CC60" s="1"/>
+      <c r="CD60" s="1"/>
     </row>
-    <row r="61" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A61" s="33" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D61" s="34" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="E61" s="2">
         <v>2</v>
@@ -10691,7 +10769,7 @@
         <v>2</v>
       </c>
       <c r="G61" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H61" s="2">
         <v>2</v>
@@ -10730,13 +10808,13 @@
         <v>1</v>
       </c>
       <c r="T61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W61" s="1">
         <v>0</v>
@@ -10808,16 +10886,16 @@
         <v>1</v>
       </c>
       <c r="AT61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV61" s="1">
         <v>1</v>
       </c>
       <c r="AW61" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX61" s="1">
         <v>0</v>
@@ -10850,7 +10928,7 @@
         <v>0</v>
       </c>
       <c r="BH61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI61" s="1">
         <v>3</v>
@@ -10875,19 +10953,20 @@
       <c r="CA61" s="1"/>
       <c r="CB61" s="1"/>
       <c r="CC61" s="1"/>
+      <c r="CD61" s="1"/>
     </row>
-    <row r="62" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D62" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E62" s="2">
         <v>2</v>
@@ -10965,7 +11044,7 @@
         <v>1</v>
       </c>
       <c r="AD62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE62" s="1">
         <v>1</v>
@@ -11013,16 +11092,16 @@
         <v>1</v>
       </c>
       <c r="AT62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV62" s="1">
         <v>1</v>
       </c>
       <c r="AW62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX62" s="1">
         <v>0</v>
@@ -11055,10 +11134,10 @@
         <v>0</v>
       </c>
       <c r="BH62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ62" s="1">
         <v>3</v>
@@ -11082,19 +11161,20 @@
       <c r="CA62" s="1"/>
       <c r="CB62" s="1"/>
       <c r="CC62" s="1"/>
+      <c r="CD62" s="1"/>
     </row>
-    <row r="63" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D63" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E63" s="2">
         <v>2</v>
@@ -11172,7 +11252,7 @@
         <v>1</v>
       </c>
       <c r="AD63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE63" s="1">
         <v>1</v>
@@ -11220,16 +11300,16 @@
         <v>1</v>
       </c>
       <c r="AT63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV63" s="1">
         <v>1</v>
       </c>
       <c r="AW63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX63" s="1">
         <v>0</v>
@@ -11262,10 +11342,10 @@
         <v>0</v>
       </c>
       <c r="BH63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ63" s="1">
         <v>0</v>
@@ -11291,19 +11371,20 @@
       <c r="CA63" s="1"/>
       <c r="CB63" s="1"/>
       <c r="CC63" s="1"/>
+      <c r="CD63" s="1"/>
     </row>
-    <row r="64" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D64" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E64" s="2">
         <v>2</v>
@@ -11381,7 +11462,7 @@
         <v>1</v>
       </c>
       <c r="AD64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE64" s="1">
         <v>1</v>
@@ -11429,16 +11510,16 @@
         <v>1</v>
       </c>
       <c r="AT64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV64" s="1">
         <v>1</v>
       </c>
       <c r="AW64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX64" s="1">
         <v>0</v>
@@ -11471,10 +11552,10 @@
         <v>0</v>
       </c>
       <c r="BH64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ64" s="1">
         <v>0</v>
@@ -11502,19 +11583,20 @@
       <c r="CA64" s="1"/>
       <c r="CB64" s="1"/>
       <c r="CC64" s="1"/>
+      <c r="CD64" s="1"/>
     </row>
-    <row r="65" spans="1:81" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D65" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E65" s="2">
         <v>2</v>
@@ -11523,7 +11605,7 @@
         <v>2</v>
       </c>
       <c r="G65" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H65" s="2">
         <v>2</v>
@@ -11562,13 +11644,13 @@
         <v>1</v>
       </c>
       <c r="T65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W65" s="1">
         <v>0</v>
@@ -11595,7 +11677,7 @@
         <v>0</v>
       </c>
       <c r="AE65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF65" s="1">
         <v>1</v>
@@ -11610,46 +11692,46 @@
         <v>1</v>
       </c>
       <c r="AJ65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL65" s="1">
         <v>1</v>
       </c>
       <c r="AM65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX65" s="1">
         <v>0</v>
@@ -11682,19 +11764,19 @@
         <v>0</v>
       </c>
       <c r="BH65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI65" s="1">
         <v>1</v>
       </c>
       <c r="BJ65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM65" s="1">
         <v>3</v>
@@ -11715,19 +11797,20 @@
       <c r="CA65" s="1"/>
       <c r="CB65" s="1"/>
       <c r="CC65" s="1"/>
+      <c r="CD65" s="1"/>
     </row>
-    <row r="66" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:82" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D66" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E66" s="2">
         <v>2</v>
@@ -11745,7 +11828,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K66" s="2">
         <v>0</v>
@@ -11763,7 +11846,7 @@
         <v>0</v>
       </c>
       <c r="P66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q66" s="1">
         <v>1</v>
@@ -11775,34 +11858,34 @@
         <v>1</v>
       </c>
       <c r="T66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W66" s="1">
         <v>0</v>
       </c>
       <c r="X66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD66" s="1">
         <v>0</v>
@@ -11814,16 +11897,16 @@
         <v>0</v>
       </c>
       <c r="AG66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK66" s="1">
         <v>0</v>
@@ -11832,7 +11915,7 @@
         <v>0</v>
       </c>
       <c r="AM66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN66" s="1">
         <v>0</v>
@@ -11856,10 +11939,10 @@
         <v>0</v>
       </c>
       <c r="AU66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW66" s="1">
         <v>0</v>
@@ -11898,19 +11981,19 @@
         <v>0</v>
       </c>
       <c r="BI66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN66" s="1">
         <v>3</v>
@@ -11930,19 +12013,20 @@
       <c r="CA66" s="1"/>
       <c r="CB66" s="1"/>
       <c r="CC66" s="1"/>
+      <c r="CD66" s="1"/>
     </row>
-    <row r="67" spans="1:81" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D67" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E67" s="2">
         <v>2</v>
@@ -12071,10 +12155,10 @@
         <v>0</v>
       </c>
       <c r="AU67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW67" s="1">
         <v>0</v>
@@ -12147,34 +12231,35 @@
       <c r="CA67" s="1"/>
       <c r="CB67" s="1"/>
       <c r="CC67" s="1"/>
+      <c r="CD67" s="1"/>
     </row>
-    <row r="68" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:82" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E68" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F68" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G68" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I68" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J68" s="1">
         <v>0</v>
@@ -12183,7 +12268,7 @@
         <v>0</v>
       </c>
       <c r="L68" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M68" s="2">
         <v>0</v>
@@ -12198,13 +12283,13 @@
         <v>0</v>
       </c>
       <c r="Q68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T68" s="1">
         <v>0</v>
@@ -12216,7 +12301,7 @@
         <v>0</v>
       </c>
       <c r="W68" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X68" s="1">
         <v>0</v>
@@ -12288,10 +12373,10 @@
         <v>0</v>
       </c>
       <c r="AU68" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW68" s="1">
         <v>0</v>
@@ -12366,19 +12451,20 @@
       <c r="CA68" s="1"/>
       <c r="CB68" s="1"/>
       <c r="CC68" s="1"/>
+      <c r="CD68" s="1"/>
     </row>
-    <row r="69" spans="1:81" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A69" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D69" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E69" s="2">
         <v>0</v>
@@ -12507,10 +12593,10 @@
         <v>0</v>
       </c>
       <c r="AU69" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW69" s="1">
         <v>0</v>
@@ -12587,19 +12673,20 @@
       <c r="CA69" s="1"/>
       <c r="CB69" s="1"/>
       <c r="CC69" s="1"/>
+      <c r="CD69" s="1"/>
     </row>
-    <row r="70" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:82" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D70" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E70" s="2">
         <v>0</v>
@@ -12623,16 +12710,16 @@
         <v>0</v>
       </c>
       <c r="L70" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M70" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N70" s="2">
         <v>0</v>
       </c>
       <c r="O70" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P70" s="2">
         <v>0</v>
@@ -12725,10 +12812,10 @@
         <v>0</v>
       </c>
       <c r="AT70" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU70" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV70" s="1">
         <v>1</v>
@@ -12810,19 +12897,20 @@
       <c r="CA70" s="1"/>
       <c r="CB70" s="1"/>
       <c r="CC70" s="1"/>
+      <c r="CD70" s="1"/>
     </row>
-    <row r="71" spans="1:81" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E71" s="2">
         <v>0</v>
@@ -12948,7 +13036,7 @@
         <v>0</v>
       </c>
       <c r="AT71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU71" s="1">
         <v>1</v>
@@ -12957,7 +13045,7 @@
         <v>1</v>
       </c>
       <c r="AW71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX71" s="1">
         <v>0</v>
@@ -13035,19 +13123,20 @@
       <c r="CA71" s="1"/>
       <c r="CB71" s="1"/>
       <c r="CC71" s="1"/>
+      <c r="CD71" s="1"/>
     </row>
-    <row r="72" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:82" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A72" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D72" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E72" s="2">
         <v>0</v>
@@ -13074,13 +13163,13 @@
         <v>0</v>
       </c>
       <c r="M72" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N72" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O72" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P72" s="2">
         <v>0</v>
@@ -13179,10 +13268,10 @@
         <v>1</v>
       </c>
       <c r="AV72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX72" s="1">
         <v>0</v>
@@ -13262,19 +13351,20 @@
       <c r="CA72" s="1"/>
       <c r="CB72" s="1"/>
       <c r="CC72" s="1"/>
+      <c r="CD72" s="1"/>
     </row>
-    <row r="73" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D73" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E73" s="2">
         <v>0</v>
@@ -13403,10 +13493,10 @@
         <v>0</v>
       </c>
       <c r="AU73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW73" s="1">
         <v>0</v>
@@ -13491,19 +13581,20 @@
       <c r="CA73" s="1"/>
       <c r="CB73" s="1"/>
       <c r="CC73" s="1"/>
+      <c r="CD73" s="1"/>
     </row>
-    <row r="74" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D74" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E74" s="2">
         <v>0</v>
@@ -13632,10 +13723,10 @@
         <v>0</v>
       </c>
       <c r="AU74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW74" s="1">
         <v>0</v>
@@ -13722,19 +13813,20 @@
       <c r="CA74" s="1"/>
       <c r="CB74" s="1"/>
       <c r="CC74" s="1"/>
+      <c r="CD74" s="1"/>
     </row>
-    <row r="75" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D75" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E75" s="2">
         <v>0</v>
@@ -13863,10 +13955,10 @@
         <v>0</v>
       </c>
       <c r="AU75" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV75" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW75" s="1">
         <v>0</v>
@@ -13955,19 +14047,20 @@
       <c r="CA75" s="1"/>
       <c r="CB75" s="1"/>
       <c r="CC75" s="1"/>
+      <c r="CD75" s="1"/>
     </row>
-    <row r="76" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E76" s="2">
         <v>0</v>
@@ -14096,10 +14189,10 @@
         <v>0</v>
       </c>
       <c r="AU76" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV76" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW76" s="1">
         <v>0</v>
@@ -14190,19 +14283,20 @@
       <c r="CA76" s="1"/>
       <c r="CB76" s="1"/>
       <c r="CC76" s="1"/>
+      <c r="CD76" s="1"/>
     </row>
-    <row r="77" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A77" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D77" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E77" s="2">
         <v>0</v>
@@ -14232,10 +14326,10 @@
         <v>0</v>
       </c>
       <c r="N77" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O77" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P77" s="2">
         <v>0</v>
@@ -14328,46 +14422,46 @@
         <v>0</v>
       </c>
       <c r="AT77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV77" s="1">
         <v>1</v>
       </c>
       <c r="AW77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH77" s="1">
         <v>0</v>
@@ -14427,19 +14521,20 @@
       <c r="CA77" s="1"/>
       <c r="CB77" s="1"/>
       <c r="CC77" s="1"/>
+      <c r="CD77" s="1"/>
     </row>
-    <row r="78" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D78" s="34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E78" s="2">
         <v>0</v>
@@ -14565,7 +14660,7 @@
         <v>0</v>
       </c>
       <c r="AT78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU78" s="1">
         <v>1</v>
@@ -14574,7 +14669,7 @@
         <v>1</v>
       </c>
       <c r="AW78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX78" s="1">
         <v>1</v>
@@ -14607,7 +14702,7 @@
         <v>1</v>
       </c>
       <c r="BH78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI78" s="1">
         <v>0</v>
@@ -14666,19 +14761,20 @@
       <c r="CA78" s="1"/>
       <c r="CB78" s="1"/>
       <c r="CC78" s="1"/>
+      <c r="CD78" s="1"/>
     </row>
-    <row r="79" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D79" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E79" s="2">
         <v>0</v>
@@ -14813,40 +14909,40 @@
         <v>1</v>
       </c>
       <c r="AW79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX79" s="1">
         <v>0</v>
       </c>
       <c r="AY79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI79" s="1">
         <v>0</v>
@@ -14907,31 +15003,32 @@
       </c>
       <c r="CB79" s="1"/>
       <c r="CC79" s="1"/>
+      <c r="CD79" s="1"/>
     </row>
-    <row r="80" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D80" s="34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E80" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F80" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I80" s="2">
         <v>2</v>
@@ -14958,22 +15055,22 @@
         <v>0</v>
       </c>
       <c r="Q80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W80" s="1">
         <v>1</v>
@@ -15048,13 +15145,13 @@
         <v>0</v>
       </c>
       <c r="AU80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV80" s="1">
         <v>1</v>
       </c>
       <c r="AW80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX80" s="1">
         <v>0</v>
@@ -15090,16 +15187,16 @@
         <v>0</v>
       </c>
       <c r="BI80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM80" s="1">
         <v>0</v>
@@ -15117,7 +15214,7 @@
         <v>0</v>
       </c>
       <c r="BR80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS80" s="1">
         <v>0</v>
@@ -15150,19 +15247,20 @@
         <v>3</v>
       </c>
       <c r="CC80" s="1"/>
+      <c r="CD80" s="1"/>
     </row>
-    <row r="81" spans="1:81" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A81" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="B81" s="36" t="s">
+    <row r="81" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A81" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C81" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D81" s="37" t="s">
-        <v>197</v>
+      <c r="C81" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D81" s="34" t="s">
+        <v>196</v>
       </c>
       <c r="E81" s="2">
         <v>2</v>
@@ -15177,7 +15275,7 @@
         <v>2</v>
       </c>
       <c r="I81" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J81" s="1">
         <v>0</v>
@@ -15195,7 +15293,7 @@
         <v>0</v>
       </c>
       <c r="O81" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P81" s="2">
         <v>0</v>
@@ -15219,7 +15317,7 @@
         <v>1</v>
       </c>
       <c r="W81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X81" s="1">
         <v>0</v>
@@ -15234,10 +15332,10 @@
         <v>0</v>
       </c>
       <c r="AB81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD81" s="1">
         <v>0</v>
@@ -15294,10 +15392,10 @@
         <v>0</v>
       </c>
       <c r="AV81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX81" s="1">
         <v>0</v>
@@ -15330,22 +15428,22 @@
         <v>0</v>
       </c>
       <c r="BH81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN81" s="1">
         <v>0</v>
@@ -15363,7 +15461,7 @@
         <v>0</v>
       </c>
       <c r="BS81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT81" s="1">
         <v>0</v>
@@ -15395,10 +15493,259 @@
       <c r="CC81" s="1">
         <v>3</v>
       </c>
+      <c r="CD81" s="1"/>
+    </row>
+    <row r="82" spans="1:82" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B82" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C82" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D82" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="E82" s="2">
+        <v>2</v>
+      </c>
+      <c r="F82" s="2">
+        <v>2</v>
+      </c>
+      <c r="G82" s="2">
+        <v>1</v>
+      </c>
+      <c r="H82" s="2">
+        <v>2</v>
+      </c>
+      <c r="I82" s="2">
+        <v>0</v>
+      </c>
+      <c r="J82" s="1">
+        <v>0</v>
+      </c>
+      <c r="K82" s="2">
+        <v>0</v>
+      </c>
+      <c r="L82" s="2">
+        <v>0</v>
+      </c>
+      <c r="M82" s="2">
+        <v>0</v>
+      </c>
+      <c r="N82" s="2">
+        <v>0</v>
+      </c>
+      <c r="O82" s="2">
+        <v>0</v>
+      </c>
+      <c r="P82" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>1</v>
+      </c>
+      <c r="R82" s="1">
+        <v>1</v>
+      </c>
+      <c r="S82" s="1">
+        <v>1</v>
+      </c>
+      <c r="T82" s="1">
+        <v>1</v>
+      </c>
+      <c r="U82" s="1">
+        <v>1</v>
+      </c>
+      <c r="V82" s="1">
+        <v>1</v>
+      </c>
+      <c r="W82" s="1">
+        <v>0</v>
+      </c>
+      <c r="X82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB82" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC82" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI82" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ82" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY82" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ82" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA82" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB82" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC82" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD82" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:CC4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A1:CC81">
+  <autoFilter ref="A4:CD4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A1:CD82">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated symbol compatibility definitions
Changes to be committed:
	modified:   qplib/data/symbols.csv
	modified:   qplib/data/symbols.xlsx
</commit_message>
<xml_diff>
--- a/qplib/data/symbols.xlsx
+++ b/qplib/data/symbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinVölkl\Desktop\qplib_dev\qplib\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A84B1A-EB19-4F33-BEB3-792AC86CBE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912EF21C-48F8-48E8-A947-A0EE5C30E5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-1920" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1433,10 +1433,10 @@
   <dimension ref="A1:CD82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="W21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z23" sqref="Z23"/>
+      <selection pane="bottomRight" activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14915,34 +14915,34 @@
         <v>0</v>
       </c>
       <c r="AY79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI79" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
qlang: added/tested invert operator
Changes to be committed:
	modified:   qplib/__pycache__/qlang.cpython-313.pyc
	modified:   qplib/data/symbols.csv
	modified:   qplib/data/symbols.xlsx
	modified:   qplib/qlang.py
	modified:   tests/__pycache__/test_qlang.cpython-313-pytest-8.3.4.pyc
	modified:   tests/test_qlang.py
</commit_message>
<xml_diff>
--- a/qplib/data/symbols.xlsx
+++ b/qplib/data/symbols.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legion16248\Desktop\data\mv\tech\qplib_dev\qplib\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinVölkl\Desktop\qplib_dev\qplib\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08394E2-69D0-4429-9F36-DAEFFEF4CEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0294239A-DCA8-4348-92D6-BB7085553CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1920" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$CD$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$CE$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="221">
   <si>
     <t>"%%"</t>
   </si>
@@ -708,6 +709,19 @@
   </si>
   <si>
     <t>trim all cols where no row values were selected</t>
+  </si>
+  <si>
+    <t>INVERT</t>
+  </si>
+  <si>
+    <t>"invert;"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invert current row selection or column selection </t>
+  </si>
+  <si>
+    <t>is any value
+(use to reset selection)</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1098,37 @@
     <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1430,96 +1474,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CD82"/>
+  <dimension ref="A1:CE83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="BG68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="Z48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BI76" sqref="BI76"/>
+      <selection pane="bottomRight" activeCell="AE63" sqref="AE63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="16" width="15.42578125" customWidth="1"/>
-    <col min="17" max="17" width="30.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="30" style="38" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="30.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="28.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="27.85546875" style="38" customWidth="1"/>
-    <col min="31" max="31" width="27.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16" style="38" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="23.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="29.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="28.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="27.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="20" style="38" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="30.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="30" style="38" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="29.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14" style="38" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="29.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="26.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="21" style="38" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="21.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="21.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="22.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="18.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="26.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="29.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="27.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="29.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="62" max="63" width="30.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="29.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="28.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="30.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="29" style="38" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="30.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="29" style="38" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="30.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="29.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="30.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="25.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="30.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="30.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="26.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="30.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="25.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="28.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="30" style="38" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="28.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="28.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.21875" style="38" customWidth="1"/>
+    <col min="18" max="19" width="26.77734375" style="38" customWidth="1"/>
+    <col min="20" max="20" width="21.21875" style="38" customWidth="1"/>
+    <col min="21" max="23" width="26.77734375" style="38" customWidth="1"/>
+    <col min="24" max="25" width="14.6640625" style="38" customWidth="1"/>
+    <col min="26" max="28" width="9.33203125" style="38" customWidth="1"/>
+    <col min="29" max="29" width="18.33203125" style="38" customWidth="1"/>
+    <col min="30" max="30" width="16.5546875" style="38" customWidth="1"/>
+    <col min="31" max="31" width="19.21875" style="2" customWidth="1"/>
+    <col min="32" max="32" width="13.77734375" style="38" customWidth="1"/>
+    <col min="33" max="33" width="11" style="38" customWidth="1"/>
+    <col min="34" max="34" width="11.88671875" style="38" customWidth="1"/>
+    <col min="35" max="36" width="11" style="38" customWidth="1"/>
+    <col min="37" max="37" width="11.88671875" style="38" customWidth="1"/>
+    <col min="38" max="38" width="12.88671875" style="38" customWidth="1"/>
+    <col min="39" max="39" width="10.5546875" style="38" customWidth="1"/>
+    <col min="40" max="40" width="11.21875" style="38" customWidth="1"/>
+    <col min="41" max="41" width="13" style="38" customWidth="1"/>
+    <col min="42" max="47" width="13.77734375" style="38" customWidth="1"/>
+    <col min="48" max="48" width="18.88671875" style="38" customWidth="1"/>
+    <col min="49" max="49" width="11.33203125" style="38" customWidth="1"/>
+    <col min="50" max="50" width="17" style="38" customWidth="1"/>
+    <col min="51" max="51" width="16.88671875" style="38" customWidth="1"/>
+    <col min="52" max="61" width="12.44140625" style="38" customWidth="1"/>
+    <col min="62" max="62" width="14.21875" style="38" customWidth="1"/>
+    <col min="63" max="63" width="26.6640625" style="38" customWidth="1"/>
+    <col min="64" max="64" width="26.109375" style="38" customWidth="1"/>
+    <col min="65" max="66" width="22.21875" style="38" customWidth="1"/>
+    <col min="67" max="67" width="24.5546875" style="38" customWidth="1"/>
+    <col min="68" max="68" width="25.109375" style="38" customWidth="1"/>
+    <col min="69" max="69" width="27.88671875" style="38" customWidth="1"/>
+    <col min="70" max="70" width="19.44140625" style="38" customWidth="1"/>
+    <col min="71" max="71" width="27" style="38" customWidth="1"/>
+    <col min="72" max="72" width="19.88671875" style="38" customWidth="1"/>
+    <col min="73" max="73" width="30.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="16" style="38" customWidth="1"/>
+    <col min="75" max="75" width="22.77734375" style="38" customWidth="1"/>
+    <col min="76" max="76" width="17.33203125" style="38" customWidth="1"/>
+    <col min="77" max="77" width="15.77734375" style="38" customWidth="1"/>
+    <col min="78" max="78" width="16.21875" style="38" customWidth="1"/>
+    <col min="79" max="79" width="13.6640625" style="38" customWidth="1"/>
+    <col min="80" max="80" width="18.5546875" style="38" customWidth="1"/>
+    <col min="81" max="81" width="15.6640625" style="38" customWidth="1"/>
+    <col min="82" max="82" width="22.44140625" style="38" customWidth="1"/>
+    <col min="83" max="83" width="17.109375" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>198</v>
@@ -1609,163 +1638,166 @@
         <v>214</v>
       </c>
       <c r="AE1" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="AF1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="AF1" s="15" t="s">
+      <c r="AG1" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AH1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AI1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AJ1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AK1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AK1" s="15" t="s">
+      <c r="AL1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="AL1" s="15" t="s">
+      <c r="AM1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AM1" s="15" t="s">
+      <c r="AN1" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="AN1" s="15" t="s">
+      <c r="AO1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="AO1" s="15" t="s">
+      <c r="AP1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="AP1" s="15" t="s">
+      <c r="AQ1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="AQ1" s="15" t="s">
+      <c r="AR1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="AR1" s="15" t="s">
+      <c r="AS1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="AS1" s="15" t="s">
+      <c r="AT1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="AT1" s="15" t="s">
+      <c r="AU1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="AU1" s="15" t="s">
+      <c r="AV1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="AV1" s="15" t="s">
+      <c r="AW1" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="AW1" s="15" t="s">
+      <c r="AX1" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="AX1" s="15" t="s">
+      <c r="AY1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="AY1" s="15" t="s">
+      <c r="AZ1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="AZ1" s="15" t="s">
+      <c r="BA1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="BA1" s="15" t="s">
+      <c r="BB1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="BB1" s="15" t="s">
+      <c r="BC1" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="BC1" s="15" t="s">
+      <c r="BD1" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="BD1" s="15" t="s">
+      <c r="BE1" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="BE1" s="15" t="s">
+      <c r="BF1" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="BF1" s="15" t="s">
+      <c r="BG1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="BG1" s="15" t="s">
+      <c r="BH1" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="BH1" s="15" t="s">
+      <c r="BI1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="BI1" s="16" t="s">
+      <c r="BJ1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="BJ1" s="16" t="s">
+      <c r="BK1" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="BK1" s="16" t="s">
+      <c r="BL1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="BL1" s="16" t="s">
+      <c r="BM1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="BM1" s="16" t="s">
+      <c r="BN1" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="BN1" s="16" t="s">
+      <c r="BO1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="BO1" s="16" t="s">
+      <c r="BP1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="BP1" s="16" t="s">
+      <c r="BQ1" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="BQ1" s="16" t="s">
+      <c r="BR1" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="BR1" s="16" t="s">
+      <c r="BS1" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="BS1" s="16" t="s">
+      <c r="BT1" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="BT1" s="16" t="s">
+      <c r="BU1" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="BU1" s="16" t="s">
+      <c r="BV1" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="BV1" s="16" t="s">
+      <c r="BW1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="BW1" s="16" t="s">
+      <c r="BX1" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="BX1" s="16" t="s">
+      <c r="BY1" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="BY1" s="16" t="s">
+      <c r="BZ1" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="BZ1" s="16" t="s">
+      <c r="CA1" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="CA1" s="16" t="s">
+      <c r="CB1" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="CB1" s="16" t="s">
+      <c r="CC1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="CC1" s="16" t="s">
+      <c r="CD1" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="CD1" s="16" t="s">
+      <c r="CE1" s="16" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:82" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>198</v>
       </c>
@@ -1946,8 +1978,8 @@
       <c r="BH2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BI2" s="5" t="s">
-        <v>67</v>
+      <c r="BI2" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="BJ2" s="5" t="s">
         <v>67</v>
@@ -2012,8 +2044,11 @@
       <c r="CD2" s="5" t="s">
         <v>67</v>
       </c>
+      <c r="CE2" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="3" spans="1:82" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:83" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>204</v>
       </c>
@@ -2077,163 +2112,166 @@
         <v>215</v>
       </c>
       <c r="AE3" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AF3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AF3" s="4" t="s">
+      <c r="AG3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AH3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AK3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AK3" s="4" t="s">
+      <c r="AL3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AM3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AM3" s="4" t="s">
+      <c r="AN3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AN3" s="4" t="s">
+      <c r="AO3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AO3" s="4" t="s">
+      <c r="AP3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AP3" s="4" t="s">
+      <c r="AQ3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AQ3" s="4" t="s">
+      <c r="AR3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AR3" s="4" t="s">
+      <c r="AS3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AS3" s="4" t="s">
+      <c r="AT3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AT3" s="4" t="s">
+      <c r="AU3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AU3" s="4" t="s">
+      <c r="AV3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AV3" s="4" t="s">
+      <c r="AW3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AW3" s="4" t="s">
+      <c r="AX3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AX3" s="4" t="s">
+      <c r="AY3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AY3" s="4" t="s">
+      <c r="AZ3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AZ3" s="4" t="s">
+      <c r="BA3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="BA3" s="4" t="s">
+      <c r="BB3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="BB3" s="4" t="s">
+      <c r="BC3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="BC3" s="4" t="s">
+      <c r="BD3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="BD3" s="4" t="s">
+      <c r="BE3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="BE3" s="4" t="s">
+      <c r="BF3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BF3" s="4" t="s">
+      <c r="BG3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="BG3" s="4" t="s">
+      <c r="BH3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BH3" s="4" t="s">
+      <c r="BI3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="BI3" s="5" t="s">
+      <c r="BJ3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="BJ3" s="5" t="s">
+      <c r="BK3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="BK3" s="5" t="s">
+      <c r="BL3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BL3" s="5" t="s">
+      <c r="BM3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="BM3" s="5" t="s">
+      <c r="BN3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="BN3" s="5" t="s">
+      <c r="BO3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="BO3" s="5" t="s">
+      <c r="BP3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="BP3" s="5" t="s">
+      <c r="BQ3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="BQ3" s="5" t="s">
+      <c r="BR3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="BR3" s="5" t="s">
+      <c r="BS3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="BS3" s="5" t="s">
+      <c r="BT3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="BT3" s="5" t="s">
+      <c r="BU3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="BU3" s="5" t="s">
+      <c r="BV3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="BV3" s="5" t="s">
+      <c r="BW3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="BW3" s="5" t="s">
+      <c r="BX3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="BX3" s="5" t="s">
+      <c r="BY3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="BY3" s="5" t="s">
+      <c r="BZ3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="BZ3" s="5" t="s">
+      <c r="CA3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="CA3" s="5" t="s">
+      <c r="CB3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="CB3" s="5" t="s">
+      <c r="CC3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="CC3" s="5" t="s">
+      <c r="CD3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="CD3" s="5" t="s">
+      <c r="CE3" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:82" s="23" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:83" s="23" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>199</v>
       </c>
@@ -2297,163 +2335,166 @@
         <v>216</v>
       </c>
       <c r="AE4" s="21" t="s">
-        <v>146</v>
+        <v>219</v>
       </c>
       <c r="AF4" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG4" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="AG4" s="21" t="s">
+      <c r="AH4" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="AH4" s="21" t="s">
+      <c r="AI4" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="AI4" s="21" t="s">
+      <c r="AJ4" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="AJ4" s="21" t="s">
+      <c r="AK4" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="AK4" s="21" t="s">
+      <c r="AL4" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="AL4" s="21" t="s">
+      <c r="AM4" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="AM4" s="21" t="s">
+      <c r="AN4" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="AN4" s="21" t="s">
+      <c r="AO4" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="AO4" s="21" t="s">
+      <c r="AP4" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="AP4" s="21" t="s">
+      <c r="AQ4" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="AQ4" s="21" t="s">
+      <c r="AR4" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="AR4" s="21" t="s">
+      <c r="AS4" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="AS4" s="21" t="s">
+      <c r="AT4" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="AT4" s="21" t="s">
+      <c r="AU4" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="AU4" s="21" t="s">
+      <c r="AV4" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="AV4" s="21" t="s">
+      <c r="AW4" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="AW4" s="21" t="s">
+      <c r="AX4" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="AX4" s="21" t="s">
+      <c r="AY4" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="AY4" s="21" t="s">
+      <c r="AZ4" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="AZ4" s="21" t="s">
+      <c r="BA4" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="BA4" s="21" t="s">
+      <c r="BB4" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="BB4" s="21" t="s">
+      <c r="BC4" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="BC4" s="21" t="s">
+      <c r="BD4" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="BD4" s="21" t="s">
+      <c r="BE4" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="BE4" s="21" t="s">
+      <c r="BF4" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="BF4" s="21" t="s">
+      <c r="BG4" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="BG4" s="21" t="s">
+      <c r="BH4" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="BH4" s="21" t="s">
+      <c r="BI4" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="BI4" s="22" t="s">
+      <c r="BJ4" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="BJ4" s="22" t="s">
+      <c r="BK4" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="BK4" s="22" t="s">
+      <c r="BL4" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="BL4" s="22" t="s">
+      <c r="BM4" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="BM4" s="22" t="s">
+      <c r="BN4" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="BN4" s="22" t="s">
+      <c r="BO4" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="BO4" s="22" t="s">
+      <c r="BP4" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="BP4" s="22" t="s">
+      <c r="BQ4" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="BQ4" s="22" t="s">
+      <c r="BR4" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="BR4" s="22" t="s">
+      <c r="BS4" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="BS4" s="22" t="s">
+      <c r="BT4" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="BT4" s="22" t="s">
+      <c r="BU4" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="BU4" s="22" t="s">
+      <c r="BV4" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="BV4" s="22" t="s">
+      <c r="BW4" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="BW4" s="22" t="s">
+      <c r="BX4" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="BX4" s="22" t="s">
+      <c r="BY4" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="BY4" s="22" t="s">
+      <c r="BZ4" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="BZ4" s="22" t="s">
+      <c r="CA4" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="CA4" s="22" t="s">
+      <c r="CB4" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="CB4" s="22" t="s">
+      <c r="CC4" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="CC4" s="22" t="s">
+      <c r="CD4" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="CD4" s="22" t="s">
+      <c r="CE4" s="22" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>201</v>
       </c>
@@ -2490,7 +2531,6 @@
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
@@ -2542,8 +2582,9 @@
       <c r="CB5" s="2"/>
       <c r="CC5" s="2"/>
       <c r="CD5" s="2"/>
+      <c r="CE5" s="2"/>
     </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>202</v>
       </c>
@@ -2582,7 +2623,6 @@
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
@@ -2634,8 +2674,9 @@
       <c r="CB6" s="2"/>
       <c r="CC6" s="2"/>
       <c r="CD6" s="2"/>
+      <c r="CE6" s="2"/>
     </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>208</v>
       </c>
@@ -2676,7 +2717,6 @@
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
@@ -2728,8 +2768,9 @@
       <c r="CB7" s="2"/>
       <c r="CC7" s="2"/>
       <c r="CD7" s="2"/>
+      <c r="CE7" s="2"/>
     </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>203</v>
       </c>
@@ -2772,7 +2813,6 @@
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
@@ -2824,8 +2864,9 @@
       <c r="CB8" s="2"/>
       <c r="CC8" s="2"/>
       <c r="CD8" s="2"/>
+      <c r="CE8" s="2"/>
     </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>207</v>
       </c>
@@ -2870,7 +2911,6 @@
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
@@ -2922,8 +2962,9 @@
       <c r="CB9" s="2"/>
       <c r="CC9" s="2"/>
       <c r="CD9" s="2"/>
+      <c r="CE9" s="2"/>
     </row>
-    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>200</v>
       </c>
@@ -2970,7 +3011,6 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
@@ -3022,8 +3062,9 @@
       <c r="CB10" s="2"/>
       <c r="CC10" s="2"/>
       <c r="CD10" s="2"/>
+      <c r="CE10" s="2"/>
     </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>205</v>
       </c>
@@ -3072,7 +3113,6 @@
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
-      <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
@@ -3124,8 +3164,9 @@
       <c r="CB11" s="2"/>
       <c r="CC11" s="2"/>
       <c r="CD11" s="2"/>
+      <c r="CE11" s="2"/>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>209</v>
       </c>
@@ -3176,7 +3217,6 @@
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
-      <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
@@ -3228,8 +3268,9 @@
       <c r="CB12" s="2"/>
       <c r="CC12" s="2"/>
       <c r="CD12" s="2"/>
+      <c r="CE12" s="2"/>
     </row>
-    <row r="13" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>210</v>
       </c>
@@ -3282,7 +3323,6 @@
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
@@ -3334,8 +3374,9 @@
       <c r="CB13" s="2"/>
       <c r="CC13" s="2"/>
       <c r="CD13" s="2"/>
+      <c r="CE13" s="2"/>
     </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>211</v>
       </c>
@@ -3390,7 +3431,6 @@
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
@@ -3442,8 +3482,9 @@
       <c r="CB14" s="2"/>
       <c r="CC14" s="2"/>
       <c r="CD14" s="2"/>
+      <c r="CE14" s="2"/>
     </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>212</v>
       </c>
@@ -3500,7 +3541,6 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
@@ -3552,8 +3592,9 @@
       <c r="CB15" s="2"/>
       <c r="CC15" s="2"/>
       <c r="CD15" s="2"/>
+      <c r="CE15" s="2"/>
     </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>213</v>
       </c>
@@ -3612,7 +3653,6 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
-      <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
@@ -3664,8 +3704,9 @@
       <c r="CB16" s="2"/>
       <c r="CC16" s="2"/>
       <c r="CD16" s="2"/>
+      <c r="CE16" s="2"/>
     </row>
-    <row r="17" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>68</v>
       </c>
@@ -3782,8 +3823,9 @@
       <c r="CB17" s="1"/>
       <c r="CC17" s="1"/>
       <c r="CD17" s="1"/>
+      <c r="CE17" s="1"/>
     </row>
-    <row r="18" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>69</v>
       </c>
@@ -3902,8 +3944,9 @@
       <c r="CB18" s="1"/>
       <c r="CC18" s="1"/>
       <c r="CD18" s="1"/>
+      <c r="CE18" s="1"/>
     </row>
-    <row r="19" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>70</v>
       </c>
@@ -4024,8 +4067,9 @@
       <c r="CB19" s="1"/>
       <c r="CC19" s="1"/>
       <c r="CD19" s="1"/>
+      <c r="CE19" s="1"/>
     </row>
-    <row r="20" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>71</v>
       </c>
@@ -4148,8 +4192,9 @@
       <c r="CB20" s="1"/>
       <c r="CC20" s="1"/>
       <c r="CD20" s="1"/>
+      <c r="CE20" s="1"/>
     </row>
-    <row r="21" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>72</v>
       </c>
@@ -4274,8 +4319,9 @@
       <c r="CB21" s="1"/>
       <c r="CC21" s="1"/>
       <c r="CD21" s="1"/>
+      <c r="CE21" s="1"/>
     </row>
-    <row r="22" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
         <v>73</v>
       </c>
@@ -4402,8 +4448,9 @@
       <c r="CB22" s="1"/>
       <c r="CC22" s="1"/>
       <c r="CD22" s="1"/>
+      <c r="CE22" s="1"/>
     </row>
-    <row r="23" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
         <v>74</v>
       </c>
@@ -4532,8 +4579,9 @@
       <c r="CB23" s="1"/>
       <c r="CC23" s="1"/>
       <c r="CD23" s="1"/>
+      <c r="CE23" s="1"/>
     </row>
-    <row r="24" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A24" s="31" t="s">
         <v>75</v>
       </c>
@@ -4664,8 +4712,9 @@
       <c r="CB24" s="1"/>
       <c r="CC24" s="1"/>
       <c r="CD24" s="1"/>
+      <c r="CE24" s="1"/>
     </row>
-    <row r="25" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
         <v>76</v>
       </c>
@@ -4798,8 +4847,9 @@
       <c r="CB25" s="1"/>
       <c r="CC25" s="1"/>
       <c r="CD25" s="1"/>
+      <c r="CE25" s="1"/>
     </row>
-    <row r="26" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
         <v>77</v>
       </c>
@@ -4934,8 +4984,9 @@
       <c r="CB26" s="1"/>
       <c r="CC26" s="1"/>
       <c r="CD26" s="1"/>
+      <c r="CE26" s="1"/>
     </row>
-    <row r="27" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>78</v>
       </c>
@@ -5072,8 +5123,9 @@
       <c r="CB27" s="1"/>
       <c r="CC27" s="1"/>
       <c r="CD27" s="1"/>
+      <c r="CE27" s="1"/>
     </row>
-    <row r="28" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A28" s="31" t="s">
         <v>79</v>
       </c>
@@ -5212,8 +5264,9 @@
       <c r="CB28" s="1"/>
       <c r="CC28" s="1"/>
       <c r="CD28" s="1"/>
+      <c r="CE28" s="1"/>
     </row>
-    <row r="29" spans="1:82" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A29" s="31" t="s">
         <v>80</v>
       </c>
@@ -5354,9 +5407,10 @@
       <c r="CB29" s="1"/>
       <c r="CC29" s="1"/>
       <c r="CD29" s="1"/>
+      <c r="CE29" s="1"/>
     </row>
-    <row r="30" spans="1:82" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
+    <row r="30" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="31" t="s">
         <v>214</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -5365,7 +5419,7 @@
       <c r="C30" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="32" t="s">
         <v>216</v>
       </c>
       <c r="E30" s="2">
@@ -5498,19 +5552,20 @@
       <c r="CB30" s="1"/>
       <c r="CC30" s="1"/>
       <c r="CD30" s="1"/>
+      <c r="CE30" s="1"/>
     </row>
-    <row r="31" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:83" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
-        <v>81</v>
+        <v>217</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>13</v>
+        <v>218</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>146</v>
+        <v>219</v>
       </c>
       <c r="E31" s="2">
         <v>2</v>
@@ -5552,19 +5607,19 @@
         <v>1</v>
       </c>
       <c r="R31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T31" s="1">
         <v>1</v>
       </c>
       <c r="U31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W31" s="1">
         <v>0</v>
@@ -5593,70 +5648,19 @@
       <c r="AE31" s="1">
         <v>3</v>
       </c>
-      <c r="AF31" s="1"/>
-      <c r="AG31" s="1"/>
-      <c r="AH31" s="1"/>
-      <c r="AI31" s="1"/>
-      <c r="AJ31" s="1"/>
-      <c r="AK31" s="1"/>
-      <c r="AL31" s="1"/>
-      <c r="AM31" s="1"/>
-      <c r="AN31" s="1"/>
-      <c r="AO31" s="1"/>
-      <c r="AP31" s="1"/>
-      <c r="AQ31" s="1"/>
-      <c r="AR31" s="1"/>
-      <c r="AS31" s="1"/>
-      <c r="AT31" s="1"/>
-      <c r="AU31" s="1"/>
-      <c r="AV31" s="1"/>
-      <c r="AW31" s="1"/>
-      <c r="AX31" s="1"/>
-      <c r="AY31" s="1"/>
-      <c r="AZ31" s="1"/>
-      <c r="BA31" s="1"/>
-      <c r="BB31" s="1"/>
-      <c r="BC31" s="1"/>
-      <c r="BD31" s="1"/>
-      <c r="BE31" s="1"/>
-      <c r="BF31" s="1"/>
-      <c r="BG31" s="1"/>
-      <c r="BH31" s="1"/>
-      <c r="BI31" s="1"/>
-      <c r="BJ31" s="1"/>
-      <c r="BK31" s="1"/>
-      <c r="BL31" s="1"/>
-      <c r="BM31" s="1"/>
-      <c r="BN31" s="1"/>
-      <c r="BO31" s="1"/>
-      <c r="BP31" s="1"/>
-      <c r="BQ31" s="1"/>
-      <c r="BR31" s="1"/>
-      <c r="BS31" s="1"/>
-      <c r="BT31" s="1"/>
-      <c r="BU31" s="1"/>
-      <c r="BV31" s="1"/>
-      <c r="BW31" s="1"/>
-      <c r="BX31" s="1"/>
-      <c r="BY31" s="1"/>
-      <c r="BZ31" s="1"/>
-      <c r="CA31" s="1"/>
-      <c r="CB31" s="1"/>
-      <c r="CC31" s="1"/>
-      <c r="CD31" s="1"/>
     </row>
-    <row r="32" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A32" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E32" s="2">
         <v>2</v>
@@ -5692,7 +5696,7 @@
         <v>0</v>
       </c>
       <c r="P32" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="1">
         <v>1</v>
@@ -5792,19 +5796,20 @@
       <c r="CB32" s="1"/>
       <c r="CC32" s="1"/>
       <c r="CD32" s="1"/>
+      <c r="CE32" s="1"/>
     </row>
-    <row r="33" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E33" s="2">
         <v>2</v>
@@ -5942,19 +5947,20 @@
       <c r="CB33" s="1"/>
       <c r="CC33" s="1"/>
       <c r="CD33" s="1"/>
+      <c r="CE33" s="1"/>
     </row>
-    <row r="34" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A34" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E34" s="2">
         <v>2</v>
@@ -6094,19 +6100,20 @@
       <c r="CB34" s="1"/>
       <c r="CC34" s="1"/>
       <c r="CD34" s="1"/>
+      <c r="CE34" s="1"/>
     </row>
-    <row r="35" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E35" s="2">
         <v>2</v>
@@ -6248,19 +6255,20 @@
       <c r="CB35" s="1"/>
       <c r="CC35" s="1"/>
       <c r="CD35" s="1"/>
+      <c r="CE35" s="1"/>
     </row>
-    <row r="36" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E36" s="2">
         <v>2</v>
@@ -6404,19 +6412,20 @@
       <c r="CB36" s="1"/>
       <c r="CC36" s="1"/>
       <c r="CD36" s="1"/>
+      <c r="CE36" s="1"/>
     </row>
-    <row r="37" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E37" s="2">
         <v>2</v>
@@ -6562,19 +6571,20 @@
       <c r="CB37" s="1"/>
       <c r="CC37" s="1"/>
       <c r="CD37" s="1"/>
+      <c r="CE37" s="1"/>
     </row>
-    <row r="38" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E38" s="2">
         <v>2</v>
@@ -6722,19 +6732,20 @@
       <c r="CB38" s="1"/>
       <c r="CC38" s="1"/>
       <c r="CD38" s="1"/>
+      <c r="CE38" s="1"/>
     </row>
-    <row r="39" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E39" s="2">
         <v>2</v>
@@ -6884,19 +6895,20 @@
       <c r="CB39" s="1"/>
       <c r="CC39" s="1"/>
       <c r="CD39" s="1"/>
+      <c r="CE39" s="1"/>
     </row>
-    <row r="40" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A40" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E40" s="2">
         <v>2</v>
@@ -6932,7 +6944,7 @@
         <v>0</v>
       </c>
       <c r="P40" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q40" s="1">
         <v>1</v>
@@ -7048,19 +7060,20 @@
       <c r="CB40" s="1"/>
       <c r="CC40" s="1"/>
       <c r="CD40" s="1"/>
+      <c r="CE40" s="1"/>
     </row>
-    <row r="41" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E41" s="2">
         <v>2</v>
@@ -7214,19 +7227,20 @@
       <c r="CB41" s="1"/>
       <c r="CC41" s="1"/>
       <c r="CD41" s="1"/>
+      <c r="CE41" s="1"/>
     </row>
-    <row r="42" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E42" s="2">
         <v>2</v>
@@ -7382,19 +7396,20 @@
       <c r="CB42" s="1"/>
       <c r="CC42" s="1"/>
       <c r="CD42" s="1"/>
+      <c r="CE42" s="1"/>
     </row>
-    <row r="43" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E43" s="2">
         <v>2</v>
@@ -7552,19 +7567,20 @@
       <c r="CB43" s="1"/>
       <c r="CC43" s="1"/>
       <c r="CD43" s="1"/>
+      <c r="CE43" s="1"/>
     </row>
-    <row r="44" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E44" s="2">
         <v>2</v>
@@ -7724,19 +7740,20 @@
       <c r="CB44" s="1"/>
       <c r="CC44" s="1"/>
       <c r="CD44" s="1"/>
+      <c r="CE44" s="1"/>
     </row>
-    <row r="45" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E45" s="2">
         <v>2</v>
@@ -7898,19 +7915,20 @@
       <c r="CB45" s="1"/>
       <c r="CC45" s="1"/>
       <c r="CD45" s="1"/>
+      <c r="CE45" s="1"/>
     </row>
-    <row r="46" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A46" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E46" s="2">
         <v>2</v>
@@ -8074,37 +8092,38 @@
       <c r="CB46" s="1"/>
       <c r="CC46" s="1"/>
       <c r="CD46" s="1"/>
+      <c r="CE46" s="1"/>
     </row>
-    <row r="47" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A47" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E47" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F47" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I47" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J47" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K47" s="2">
         <v>0</v>
@@ -8119,31 +8138,31 @@
         <v>0</v>
       </c>
       <c r="O47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P47" s="2">
         <v>0</v>
       </c>
       <c r="Q47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X47" s="1">
         <v>0</v>
@@ -8252,19 +8271,20 @@
       <c r="CB47" s="1"/>
       <c r="CC47" s="1"/>
       <c r="CD47" s="1"/>
+      <c r="CE47" s="1"/>
     </row>
-    <row r="48" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E48" s="2">
         <v>0</v>
@@ -8288,10 +8308,10 @@
         <v>0</v>
       </c>
       <c r="L48" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M48" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N48" s="2">
         <v>0</v>
@@ -8303,22 +8323,22 @@
         <v>0</v>
       </c>
       <c r="Q48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W48" s="1">
         <v>1</v>
@@ -8432,31 +8452,32 @@
       <c r="CB48" s="1"/>
       <c r="CC48" s="1"/>
       <c r="CD48" s="1"/>
+      <c r="CE48" s="1"/>
     </row>
-    <row r="49" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E49" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F49" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G49" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I49" s="2">
         <v>2</v>
@@ -8468,10 +8489,10 @@
         <v>0</v>
       </c>
       <c r="L49" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M49" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N49" s="2">
         <v>0</v>
@@ -8614,37 +8635,38 @@
       <c r="CB49" s="1"/>
       <c r="CC49" s="1"/>
       <c r="CD49" s="1"/>
+      <c r="CE49" s="1"/>
     </row>
-    <row r="50" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A50" s="31" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="E50" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F50" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I50" s="2">
         <v>2</v>
       </c>
       <c r="J50" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K50" s="2">
         <v>0</v>
@@ -8665,22 +8687,22 @@
         <v>0</v>
       </c>
       <c r="Q50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W50" s="1">
         <v>1</v>
@@ -8798,19 +8820,20 @@
       <c r="CB50" s="1"/>
       <c r="CC50" s="1"/>
       <c r="CD50" s="1"/>
+      <c r="CE50" s="1"/>
     </row>
-    <row r="51" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E51" s="2">
         <v>0</v>
@@ -8831,7 +8854,7 @@
         <v>2</v>
       </c>
       <c r="K51" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L51" s="2">
         <v>0</v>
@@ -8984,19 +9007,20 @@
       <c r="CB51" s="1"/>
       <c r="CC51" s="1"/>
       <c r="CD51" s="1"/>
+      <c r="CE51" s="1"/>
     </row>
-    <row r="52" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A52" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E52" s="2">
         <v>0</v>
@@ -9172,19 +9196,20 @@
       <c r="CB52" s="1"/>
       <c r="CC52" s="1"/>
       <c r="CD52" s="1"/>
+      <c r="CE52" s="1"/>
     </row>
-    <row r="53" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E53" s="2">
         <v>0</v>
@@ -9362,19 +9387,20 @@
       <c r="CB53" s="1"/>
       <c r="CC53" s="1"/>
       <c r="CD53" s="1"/>
+      <c r="CE53" s="1"/>
     </row>
-    <row r="54" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E54" s="2">
         <v>0</v>
@@ -9554,19 +9580,20 @@
       <c r="CB54" s="1"/>
       <c r="CC54" s="1"/>
       <c r="CD54" s="1"/>
+      <c r="CE54" s="1"/>
     </row>
-    <row r="55" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A55" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E55" s="2">
         <v>0</v>
@@ -9748,19 +9775,20 @@
       <c r="CB55" s="1"/>
       <c r="CC55" s="1"/>
       <c r="CD55" s="1"/>
+      <c r="CE55" s="1"/>
     </row>
-    <row r="56" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A56" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E56" s="2">
         <v>0</v>
@@ -9944,19 +9972,20 @@
       <c r="CB56" s="1"/>
       <c r="CC56" s="1"/>
       <c r="CD56" s="1"/>
+      <c r="CE56" s="1"/>
     </row>
-    <row r="57" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A57" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E57" s="2">
         <v>0</v>
@@ -10142,19 +10171,20 @@
       <c r="CB57" s="1"/>
       <c r="CC57" s="1"/>
       <c r="CD57" s="1"/>
+      <c r="CE57" s="1"/>
     </row>
-    <row r="58" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A58" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E58" s="2">
         <v>0</v>
@@ -10342,19 +10372,20 @@
       <c r="CB58" s="1"/>
       <c r="CC58" s="1"/>
       <c r="CD58" s="1"/>
+      <c r="CE58" s="1"/>
     </row>
-    <row r="59" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A59" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
@@ -10544,19 +10575,20 @@
       <c r="CB59" s="1"/>
       <c r="CC59" s="1"/>
       <c r="CD59" s="1"/>
+      <c r="CE59" s="1"/>
     </row>
-    <row r="60" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A60" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D60" s="32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E60" s="2">
         <v>0</v>
@@ -10748,40 +10780,41 @@
       <c r="CB60" s="1"/>
       <c r="CC60" s="1"/>
       <c r="CD60" s="1"/>
+      <c r="CE60" s="1"/>
     </row>
-    <row r="61" spans="1:82" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D61" s="34" t="s">
-        <v>180</v>
+    <row r="61" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="A61" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>173</v>
       </c>
       <c r="E61" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F61" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I61" s="2">
-        <v>1</v>
-      </c>
-      <c r="J61" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J61" s="2">
+        <v>2</v>
       </c>
       <c r="K61" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L61" s="2">
         <v>0</v>
@@ -10793,112 +10826,112 @@
         <v>0</v>
       </c>
       <c r="O61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P61" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W61" s="1">
         <v>1</v>
       </c>
       <c r="X61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU61" s="1">
         <v>0</v>
       </c>
       <c r="AV61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY61" s="1">
         <v>0</v>
@@ -10954,19 +10987,20 @@
       <c r="CB61" s="1"/>
       <c r="CC61" s="1"/>
       <c r="CD61" s="1"/>
+      <c r="CE61" s="1"/>
     </row>
-    <row r="62" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A62" s="33" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D62" s="34" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="E62" s="2">
         <v>2</v>
@@ -10975,13 +11009,13 @@
         <v>2</v>
       </c>
       <c r="G62" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H62" s="2">
         <v>2</v>
       </c>
       <c r="I62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" s="1">
         <v>1</v>
@@ -11014,16 +11048,16 @@
         <v>1</v>
       </c>
       <c r="T62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X62" s="1">
         <v>1</v>
@@ -11044,10 +11078,10 @@
         <v>1</v>
       </c>
       <c r="AD62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF62" s="1">
         <v>1</v>
@@ -11095,19 +11129,19 @@
         <v>1</v>
       </c>
       <c r="AU62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW62" s="1">
         <v>1</v>
       </c>
       <c r="AX62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ62" s="1">
         <v>0</v>
@@ -11137,7 +11171,7 @@
         <v>0</v>
       </c>
       <c r="BI62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ62" s="1">
         <v>3</v>
@@ -11162,19 +11196,20 @@
       <c r="CB62" s="1"/>
       <c r="CC62" s="1"/>
       <c r="CD62" s="1"/>
+      <c r="CE62" s="1"/>
     </row>
-    <row r="63" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D63" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E63" s="2">
         <v>2</v>
@@ -11303,16 +11338,16 @@
         <v>1</v>
       </c>
       <c r="AU63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW63" s="1">
         <v>1</v>
       </c>
       <c r="AX63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY63" s="1">
         <v>0</v>
@@ -11345,10 +11380,10 @@
         <v>0</v>
       </c>
       <c r="BI63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK63" s="1">
         <v>3</v>
@@ -11372,19 +11407,20 @@
       <c r="CB63" s="1"/>
       <c r="CC63" s="1"/>
       <c r="CD63" s="1"/>
+      <c r="CE63" s="1"/>
     </row>
-    <row r="64" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D64" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E64" s="2">
         <v>2</v>
@@ -11513,16 +11549,16 @@
         <v>1</v>
       </c>
       <c r="AU64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW64" s="1">
         <v>1</v>
       </c>
       <c r="AX64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY64" s="1">
         <v>0</v>
@@ -11555,10 +11591,10 @@
         <v>0</v>
       </c>
       <c r="BI64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK64" s="1">
         <v>0</v>
@@ -11584,19 +11620,20 @@
       <c r="CB64" s="1"/>
       <c r="CC64" s="1"/>
       <c r="CD64" s="1"/>
+      <c r="CE64" s="1"/>
     </row>
-    <row r="65" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D65" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E65" s="2">
         <v>2</v>
@@ -11725,16 +11762,16 @@
         <v>1</v>
       </c>
       <c r="AU65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW65" s="1">
         <v>1</v>
       </c>
       <c r="AX65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY65" s="1">
         <v>0</v>
@@ -11767,10 +11804,10 @@
         <v>0</v>
       </c>
       <c r="BI65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK65" s="1">
         <v>0</v>
@@ -11798,19 +11835,20 @@
       <c r="CB65" s="1"/>
       <c r="CC65" s="1"/>
       <c r="CD65" s="1"/>
+      <c r="CE65" s="1"/>
     </row>
-    <row r="66" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D66" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E66" s="2">
         <v>2</v>
@@ -11819,7 +11857,7 @@
         <v>2</v>
       </c>
       <c r="G66" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H66" s="2">
         <v>2</v>
@@ -11858,13 +11896,13 @@
         <v>1</v>
       </c>
       <c r="T66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W66" s="1">
         <v>0</v>
@@ -11891,10 +11929,10 @@
         <v>0</v>
       </c>
       <c r="AE66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG66" s="1">
         <v>1</v>
@@ -11909,46 +11947,46 @@
         <v>1</v>
       </c>
       <c r="AK66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM66" s="1">
         <v>1</v>
       </c>
       <c r="AN66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX66" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY66" s="1">
         <v>0</v>
@@ -11981,19 +12019,19 @@
         <v>0</v>
       </c>
       <c r="BI66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ66" s="1">
         <v>1</v>
       </c>
       <c r="BK66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN66" s="1">
         <v>3</v>
@@ -12014,19 +12052,20 @@
       <c r="CB66" s="1"/>
       <c r="CC66" s="1"/>
       <c r="CD66" s="1"/>
+      <c r="CE66" s="1"/>
     </row>
-    <row r="67" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D67" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E67" s="2">
         <v>2</v>
@@ -12044,7 +12083,7 @@
         <v>0</v>
       </c>
       <c r="J67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K67" s="2">
         <v>0</v>
@@ -12062,7 +12101,7 @@
         <v>0</v>
       </c>
       <c r="P67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q67" s="1">
         <v>1</v>
@@ -12074,34 +12113,34 @@
         <v>1</v>
       </c>
       <c r="T67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W67" s="1">
         <v>0</v>
       </c>
       <c r="X67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD67" s="1">
         <v>0</v>
@@ -12116,16 +12155,16 @@
         <v>0</v>
       </c>
       <c r="AH67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL67" s="1">
         <v>0</v>
@@ -12134,7 +12173,7 @@
         <v>0</v>
       </c>
       <c r="AN67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO67" s="1">
         <v>0</v>
@@ -12158,10 +12197,10 @@
         <v>0</v>
       </c>
       <c r="AV67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX67" s="1">
         <v>0</v>
@@ -12200,19 +12239,19 @@
         <v>0</v>
       </c>
       <c r="BJ67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO67" s="1">
         <v>3</v>
@@ -12232,19 +12271,20 @@
       <c r="CB67" s="1"/>
       <c r="CC67" s="1"/>
       <c r="CD67" s="1"/>
+      <c r="CE67" s="1"/>
     </row>
-    <row r="68" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E68" s="2">
         <v>2</v>
@@ -12376,10 +12416,10 @@
         <v>0</v>
       </c>
       <c r="AV68" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX68" s="1">
         <v>0</v>
@@ -12452,34 +12492,35 @@
       <c r="CB68" s="1"/>
       <c r="CC68" s="1"/>
       <c r="CD68" s="1"/>
+      <c r="CE68" s="1"/>
     </row>
-    <row r="69" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D69" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E69" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F69" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I69" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J69" s="1">
         <v>0</v>
@@ -12488,7 +12529,7 @@
         <v>0</v>
       </c>
       <c r="L69" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M69" s="2">
         <v>0</v>
@@ -12503,13 +12544,13 @@
         <v>0</v>
       </c>
       <c r="Q69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T69" s="1">
         <v>0</v>
@@ -12521,7 +12562,7 @@
         <v>0</v>
       </c>
       <c r="W69" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X69" s="1">
         <v>0</v>
@@ -12596,10 +12637,10 @@
         <v>0</v>
       </c>
       <c r="AV69" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX69" s="1">
         <v>0</v>
@@ -12674,19 +12715,20 @@
       <c r="CB69" s="1"/>
       <c r="CC69" s="1"/>
       <c r="CD69" s="1"/>
+      <c r="CE69" s="1"/>
     </row>
-    <row r="70" spans="1:82" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A70" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D70" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E70" s="2">
         <v>0</v>
@@ -12818,10 +12860,10 @@
         <v>0</v>
       </c>
       <c r="AV70" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW70" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX70" s="1">
         <v>0</v>
@@ -12898,19 +12940,20 @@
       <c r="CB70" s="1"/>
       <c r="CC70" s="1"/>
       <c r="CD70" s="1"/>
+      <c r="CE70" s="1"/>
     </row>
-    <row r="71" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:83" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E71" s="2">
         <v>0</v>
@@ -12934,16 +12977,16 @@
         <v>0</v>
       </c>
       <c r="L71" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M71" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N71" s="2">
         <v>0</v>
       </c>
       <c r="O71" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P71" s="2">
         <v>0</v>
@@ -13039,10 +13082,10 @@
         <v>0</v>
       </c>
       <c r="AU71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW71" s="1">
         <v>1</v>
@@ -13124,19 +13167,20 @@
       <c r="CB71" s="1"/>
       <c r="CC71" s="1"/>
       <c r="CD71" s="1"/>
+      <c r="CE71" s="1"/>
     </row>
-    <row r="72" spans="1:82" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D72" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E72" s="2">
         <v>0</v>
@@ -13265,7 +13309,7 @@
         <v>0</v>
       </c>
       <c r="AU72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV72" s="1">
         <v>1</v>
@@ -13274,7 +13318,7 @@
         <v>1</v>
       </c>
       <c r="AX72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY72" s="1">
         <v>0</v>
@@ -13352,19 +13396,20 @@
       <c r="CB72" s="1"/>
       <c r="CC72" s="1"/>
       <c r="CD72" s="1"/>
+      <c r="CE72" s="1"/>
     </row>
-    <row r="73" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:83" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A73" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D73" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E73" s="2">
         <v>0</v>
@@ -13391,13 +13436,13 @@
         <v>0</v>
       </c>
       <c r="M73" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N73" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O73" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P73" s="2">
         <v>0</v>
@@ -13499,10 +13544,10 @@
         <v>1</v>
       </c>
       <c r="AW73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY73" s="1">
         <v>0</v>
@@ -13582,19 +13627,20 @@
       <c r="CB73" s="1"/>
       <c r="CC73" s="1"/>
       <c r="CD73" s="1"/>
+      <c r="CE73" s="1"/>
     </row>
-    <row r="74" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D74" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E74" s="2">
         <v>0</v>
@@ -13726,10 +13772,10 @@
         <v>0</v>
       </c>
       <c r="AV74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX74" s="1">
         <v>0</v>
@@ -13814,19 +13860,20 @@
       <c r="CB74" s="1"/>
       <c r="CC74" s="1"/>
       <c r="CD74" s="1"/>
+      <c r="CE74" s="1"/>
     </row>
-    <row r="75" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D75" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E75" s="2">
         <v>0</v>
@@ -13958,10 +14005,10 @@
         <v>0</v>
       </c>
       <c r="AV75" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW75" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX75" s="1">
         <v>0</v>
@@ -14048,19 +14095,20 @@
       <c r="CB75" s="1"/>
       <c r="CC75" s="1"/>
       <c r="CD75" s="1"/>
+      <c r="CE75" s="1"/>
     </row>
-    <row r="76" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E76" s="2">
         <v>0</v>
@@ -14192,10 +14240,10 @@
         <v>0</v>
       </c>
       <c r="AV76" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW76" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX76" s="1">
         <v>0</v>
@@ -14284,19 +14332,20 @@
       <c r="CB76" s="1"/>
       <c r="CC76" s="1"/>
       <c r="CD76" s="1"/>
+      <c r="CE76" s="1"/>
     </row>
-    <row r="77" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D77" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E77" s="2">
         <v>0</v>
@@ -14428,10 +14477,10 @@
         <v>0</v>
       </c>
       <c r="AV77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX77" s="1">
         <v>0</v>
@@ -14522,19 +14571,20 @@
       <c r="CB77" s="1"/>
       <c r="CC77" s="1"/>
       <c r="CD77" s="1"/>
+      <c r="CE77" s="1"/>
     </row>
-    <row r="78" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D78" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E78" s="2">
         <v>0</v>
@@ -14564,10 +14614,10 @@
         <v>0</v>
       </c>
       <c r="N78" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O78" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P78" s="2">
         <v>0</v>
@@ -14663,49 +14713,49 @@
         <v>0</v>
       </c>
       <c r="AU78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW78" s="1">
         <v>1</v>
       </c>
       <c r="AX78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ78" s="1">
         <v>0</v>
@@ -14762,19 +14812,20 @@
       <c r="CB78" s="1"/>
       <c r="CC78" s="1"/>
       <c r="CD78" s="1"/>
+      <c r="CE78" s="1"/>
     </row>
-    <row r="79" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A79" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D79" s="34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E79" s="2">
         <v>0</v>
@@ -14903,7 +14954,7 @@
         <v>0</v>
       </c>
       <c r="AU79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV79" s="1">
         <v>1</v>
@@ -14912,43 +14963,43 @@
         <v>1</v>
       </c>
       <c r="AX79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK79" s="1">
         <v>0</v>
@@ -15004,19 +15055,20 @@
       <c r="CB79" s="1"/>
       <c r="CC79" s="1"/>
       <c r="CD79" s="1"/>
+      <c r="CE79" s="1"/>
     </row>
-    <row r="80" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D80" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E80" s="2">
         <v>0</v>
@@ -15154,7 +15206,7 @@
         <v>1</v>
       </c>
       <c r="AX80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY80" s="1">
         <v>0</v>
@@ -15248,31 +15300,32 @@
       </c>
       <c r="CC80" s="1"/>
       <c r="CD80" s="1"/>
+      <c r="CE80" s="1"/>
     </row>
-    <row r="81" spans="1:82" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D81" s="34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E81" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F81" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G81" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I81" s="2">
         <v>2</v>
@@ -15299,22 +15352,22 @@
         <v>0</v>
       </c>
       <c r="Q81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W81" s="1">
         <v>1</v>
@@ -15392,13 +15445,13 @@
         <v>0</v>
       </c>
       <c r="AV81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW81" s="1">
         <v>1</v>
       </c>
       <c r="AX81" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY81" s="1">
         <v>0</v>
@@ -15434,16 +15487,16 @@
         <v>0</v>
       </c>
       <c r="BJ81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN81" s="1">
         <v>0</v>
@@ -15461,7 +15514,7 @@
         <v>0</v>
       </c>
       <c r="BS81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT81" s="1">
         <v>0</v>
@@ -15494,19 +15547,20 @@
         <v>3</v>
       </c>
       <c r="CD81" s="1"/>
+      <c r="CE81" s="1"/>
     </row>
-    <row r="82" spans="1:82" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="B82" s="36" t="s">
+    <row r="82" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C82" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D82" s="37" t="s">
-        <v>197</v>
+      <c r="C82" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D82" s="34" t="s">
+        <v>196</v>
       </c>
       <c r="E82" s="2">
         <v>2</v>
@@ -15521,7 +15575,7 @@
         <v>2</v>
       </c>
       <c r="I82" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J82" s="1">
         <v>0</v>
@@ -15539,7 +15593,7 @@
         <v>0</v>
       </c>
       <c r="O82" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P82" s="2">
         <v>0</v>
@@ -15563,7 +15617,7 @@
         <v>1</v>
       </c>
       <c r="W82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X82" s="1">
         <v>0</v>
@@ -15578,10 +15632,10 @@
         <v>0</v>
       </c>
       <c r="AB82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD82" s="1">
         <v>0</v>
@@ -15641,10 +15695,10 @@
         <v>0</v>
       </c>
       <c r="AW82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY82" s="1">
         <v>0</v>
@@ -15677,22 +15731,22 @@
         <v>0</v>
       </c>
       <c r="BI82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO82" s="1">
         <v>0</v>
@@ -15710,7 +15764,7 @@
         <v>0</v>
       </c>
       <c r="BT82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU82" s="1">
         <v>0</v>
@@ -15742,21 +15796,298 @@
       <c r="CD82" s="1">
         <v>3</v>
       </c>
+      <c r="CE82" s="1"/>
+    </row>
+    <row r="83" spans="1:83" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A83" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B83" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C83" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D83" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="E83" s="2">
+        <v>2</v>
+      </c>
+      <c r="F83" s="2">
+        <v>2</v>
+      </c>
+      <c r="G83" s="2">
+        <v>1</v>
+      </c>
+      <c r="H83" s="2">
+        <v>2</v>
+      </c>
+      <c r="I83" s="2">
+        <v>0</v>
+      </c>
+      <c r="J83" s="1">
+        <v>0</v>
+      </c>
+      <c r="K83" s="2">
+        <v>0</v>
+      </c>
+      <c r="L83" s="2">
+        <v>0</v>
+      </c>
+      <c r="M83" s="2">
+        <v>0</v>
+      </c>
+      <c r="N83" s="2">
+        <v>0</v>
+      </c>
+      <c r="O83" s="2">
+        <v>0</v>
+      </c>
+      <c r="P83" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="1">
+        <v>1</v>
+      </c>
+      <c r="R83" s="1">
+        <v>1</v>
+      </c>
+      <c r="S83" s="1">
+        <v>1</v>
+      </c>
+      <c r="T83" s="1">
+        <v>1</v>
+      </c>
+      <c r="U83" s="1">
+        <v>1</v>
+      </c>
+      <c r="V83" s="1">
+        <v>1</v>
+      </c>
+      <c r="W83" s="1">
+        <v>0</v>
+      </c>
+      <c r="X83" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y83" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB83" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC83" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY83" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ83" s="1">
+        <v>1</v>
+      </c>
+      <c r="BK83" s="1">
+        <v>1</v>
+      </c>
+      <c r="BL83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY83" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ83" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA83" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB83" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC83" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD83" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE83" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:CD4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A1:CD82">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <autoFilter ref="A4:CE4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A31:D31">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:CE83">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD43F287-0BDC-4CE3-B4F1-F401FA5BE851}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
qlang: testing modification scope changes (wip)
Changes to be committed:
	modified:   interactive_demo.ipynb
	modified:   qplib/__pycache__/qlang.cpython-313.pyc
	modified:   qplib/data/symbols.csv
	modified:   qplib/data/symbols.xlsx
	modified:   qplib/qlang.py
	modified:   tests/__pycache__/test_qlang.cpython-313-pytest-8.3.4.pyc
	modified:   tests/test_qlang.py
</commit_message>
<xml_diff>
--- a/qplib/data/symbols.xlsx
+++ b/qplib/data/symbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinVölkl\Desktop\qplib_dev\qplib\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1D5DB0-031B-46CD-ADEF-46673A575337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD8F2BD-CE27-4F16-B899-BA756F4AB363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$CH$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$CI$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="231">
   <si>
     <t>"%%"</t>
   </si>
@@ -236,12 +236,6 @@
     <t>"css"</t>
   </si>
   <si>
-    <t>"val"</t>
-  </si>
-  <si>
-    <t>"header"</t>
-  </si>
-  <si>
     <t>"new"</t>
   </si>
   <si>
@@ -437,12 +431,6 @@
     <t>CSS</t>
   </si>
   <si>
-    <t>VAL</t>
-  </si>
-  <si>
-    <t>HEADER</t>
-  </si>
-  <si>
     <t>NEW_COL</t>
   </si>
   <si>
@@ -630,9 +618,6 @@
   </si>
   <si>
     <t>modify selected values</t>
-  </si>
-  <si>
-    <t>modify the headers of the selected columns</t>
   </si>
   <si>
     <t>create a new column with the selected values</t>
@@ -742,6 +727,30 @@
   </si>
   <si>
     <t>trim row/col selection based on val selection.</t>
+  </si>
+  <si>
+    <t>"vals"</t>
+  </si>
+  <si>
+    <t>"cols"</t>
+  </si>
+  <si>
+    <t>COLS</t>
+  </si>
+  <si>
+    <t>modify the colnames of the selected columns</t>
+  </si>
+  <si>
+    <t>VALS</t>
+  </si>
+  <si>
+    <t>ROWS</t>
+  </si>
+  <si>
+    <t>"rows"</t>
+  </si>
+  <si>
+    <t>modify the values in the selected rows</t>
   </si>
 </sst>
 </file>
@@ -1464,13 +1473,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CI86"/>
+  <dimension ref="A1:CI87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="T68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="BX75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Y71" sqref="Y71"/>
+      <selection pane="bottomRight" activeCell="CG81" sqref="CG81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,537 +1543,543 @@
     <col min="79" max="79" width="17.28515625" style="38" customWidth="1"/>
     <col min="80" max="80" width="15.7109375" style="38" customWidth="1"/>
     <col min="81" max="81" width="16.28515625" style="38" customWidth="1"/>
-    <col min="82" max="82" width="13.7109375" style="38" customWidth="1"/>
-    <col min="83" max="83" width="18.5703125" style="38" customWidth="1"/>
-    <col min="84" max="84" width="15.7109375" style="38" customWidth="1"/>
-    <col min="85" max="85" width="22.42578125" style="38" customWidth="1"/>
-    <col min="86" max="86" width="17.140625" style="38" customWidth="1"/>
+    <col min="82" max="82" width="18.5703125" style="38" customWidth="1"/>
+    <col min="83" max="84" width="13.7109375" style="38" customWidth="1"/>
+    <col min="85" max="85" width="15.7109375" style="38" customWidth="1"/>
+    <col min="86" max="86" width="22.42578125" style="38" customWidth="1"/>
+    <col min="87" max="87" width="17.140625" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:87" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="J1" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="N1" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB1" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD1" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE1" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF1" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG1" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH1" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="AI1" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="AJ1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK1" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL1" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM1" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO1" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP1" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AU1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="AV1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="AY1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="BA1" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="BB1" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="BC1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD1" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="BE1" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="BF1" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="BG1" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="BH1" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="BI1" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="BJ1" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="BK1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="BL1" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="BM1" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="BN1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="BO1" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="BQ1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="BR1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BS1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BT1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="BU1" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="BV1" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="BW1" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="BX1" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="BY1" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="BZ1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="CA1" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="CB1" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="CC1" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="CD1" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="CE1" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="CF1" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="CG1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="CH1" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="CI1" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:87" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BB2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BC2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BD2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BG2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BI2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BJ2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BL2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BP2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BQ2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BR2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BS2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BT2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BU2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BV2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BW2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BX2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BY2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BZ2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="CA2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="CB2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="CC2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="CD2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="CE2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="CF2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="CG2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="CH2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="CI2" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:87" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="B3" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="T1" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="V1" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="W1" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="X1" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y1" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z1" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB1" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC1" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD1" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE1" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF1" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="AG1" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH1" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="AJ1" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK1" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="AL1" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM1" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN1" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="AO1" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="AP1" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="AQ1" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR1" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="AS1" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="AT1" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU1" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV1" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AW1" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="AX1" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="AY1" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="AZ1" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="BA1" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="BB1" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="BC1" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="BD1" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="BE1" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="BF1" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="BG1" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="BH1" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="BI1" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="BJ1" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="BK1" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="BL1" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="BM1" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="BN1" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="BO1" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="BP1" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="BQ1" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="BR1" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="BS1" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="BT1" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="BU1" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="BV1" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="BW1" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="BX1" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="BY1" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="BZ1" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="CA1" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="CB1" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="CC1" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="CD1" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="CE1" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="CF1" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="CG1" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="CH1" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:86" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AO2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AP2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AQ2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AR2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AV2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AW2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AX2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AY2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AZ2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BA2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BB2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BC2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BD2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BE2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BF2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BG2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BH2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BI2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BJ2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BK2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BL2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BM2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="BN2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BO2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BP2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BQ2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BR2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BS2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BT2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BU2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BV2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BW2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BX2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BY2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BZ2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="CA2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="CB2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="CC2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="CD2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="CE2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="CF2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="CG2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="CH2" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:86" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>203</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="9"/>
@@ -2082,13 +2097,13 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>0</v>
@@ -2130,10 +2145,10 @@
         <v>12</v>
       </c>
       <c r="AH3" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="AI3" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AJ3" s="4" t="s">
         <v>13</v>
@@ -2274,27 +2289,30 @@
         <v>58</v>
       </c>
       <c r="CD3" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="CE3" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="CF3" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="CG3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="CE3" s="5" t="s">
+      <c r="CH3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="CF3" s="5" t="s">
+      <c r="CI3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="CG3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="CH3" s="5" t="s">
-        <v>63</v>
-      </c>
     </row>
-    <row r="4" spans="1:86" s="23" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:87" s="23" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="9"/>
@@ -2312,219 +2330,222 @@
       <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
       <c r="R4" s="20" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="S4" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="V4" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="W4" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="X4" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y4" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z4" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA4" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB4" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC4" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD4" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF4" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG4" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="AH4" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="T4" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="U4" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="V4" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="W4" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="X4" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y4" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z4" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="AA4" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB4" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="AC4" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="AD4" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE4" s="21" t="s">
+      <c r="AI4" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ4" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="AK4" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="AF4" s="21" t="s">
+      <c r="AL4" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="AG4" s="21" t="s">
+      <c r="AM4" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="AH4" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="AI4" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="AJ4" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="AK4" s="21" t="s">
+      <c r="AN4" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO4" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="AL4" s="21" t="s">
+      <c r="AP4" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="AM4" s="21" t="s">
+      <c r="AQ4" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="AN4" s="21" t="s">
+      <c r="AR4" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="AO4" s="21" t="s">
+      <c r="AS4" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="AP4" s="21" t="s">
+      <c r="AT4" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="AQ4" s="21" t="s">
+      <c r="AU4" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="AR4" s="21" t="s">
+      <c r="AV4" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="AS4" s="21" t="s">
+      <c r="AW4" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="AT4" s="21" t="s">
+      <c r="AX4" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="AU4" s="21" t="s">
+      <c r="AY4" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="AV4" s="21" t="s">
+      <c r="AZ4" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="AW4" s="21" t="s">
+      <c r="BA4" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="BB4" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="BC4" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="AX4" s="21" t="s">
+      <c r="BD4" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="AY4" s="21" t="s">
+      <c r="BE4" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="AZ4" s="21" t="s">
+      <c r="BF4" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="BA4" s="21" t="s">
+      <c r="BG4" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="BH4" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="BI4" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="BJ4" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="BK4" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="BL4" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="BM4" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="BN4" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="BO4" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="BP4" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="BQ4" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="BB4" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="BC4" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="BD4" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="BE4" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="BF4" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="BG4" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="BH4" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="BI4" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="BJ4" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BK4" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="BL4" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="BM4" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="BN4" s="22" t="s">
+      <c r="BR4" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="BS4" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="BT4" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="BU4" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="BO4" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="BP4" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="BQ4" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="BR4" s="22" t="s">
+      <c r="BV4" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="BS4" s="22" t="s">
+      <c r="BW4" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="BT4" s="22" t="s">
+      <c r="BX4" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="BU4" s="22" t="s">
+      <c r="BY4" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="BV4" s="22" t="s">
+      <c r="BZ4" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="BW4" s="22" t="s">
+      <c r="CA4" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="BX4" s="22" t="s">
+      <c r="CB4" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="BY4" s="22" t="s">
+      <c r="CC4" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="BZ4" s="22" t="s">
+      <c r="CD4" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="CE4" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF4" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="CA4" s="22" t="s">
+      <c r="CG4" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="CB4" s="22" t="s">
+      <c r="CH4" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="CC4" s="22" t="s">
+      <c r="CI4" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="CD4" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="CE4" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="CF4" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="CG4" s="22" t="s">
+    </row>
+    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="CH4" s="22" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="B5" s="12" t="s">
         <v>198</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>203</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="28"/>
@@ -2611,13 +2632,14 @@
       <c r="CF5" s="2"/>
       <c r="CG5" s="2"/>
       <c r="CH5" s="2"/>
+      <c r="CI5" s="2"/>
     </row>
-    <row r="6" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="26"/>
@@ -2706,13 +2728,14 @@
       <c r="CF6" s="2"/>
       <c r="CG6" s="2"/>
       <c r="CH6" s="2"/>
+      <c r="CI6" s="2"/>
     </row>
-    <row r="7" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="26"/>
@@ -2803,13 +2826,14 @@
       <c r="CF7" s="2"/>
       <c r="CG7" s="2"/>
       <c r="CH7" s="2"/>
+      <c r="CI7" s="2"/>
     </row>
-    <row r="8" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="26"/>
@@ -2902,13 +2926,14 @@
       <c r="CF8" s="2"/>
       <c r="CG8" s="2"/>
       <c r="CH8" s="2"/>
+      <c r="CI8" s="2"/>
     </row>
-    <row r="9" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="26"/>
@@ -3003,13 +3028,14 @@
       <c r="CF9" s="2"/>
       <c r="CG9" s="2"/>
       <c r="CH9" s="2"/>
+      <c r="CI9" s="2"/>
     </row>
-    <row r="10" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="26"/>
@@ -3106,13 +3132,14 @@
       <c r="CF10" s="2"/>
       <c r="CG10" s="2"/>
       <c r="CH10" s="2"/>
+      <c r="CI10" s="2"/>
     </row>
-    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="26"/>
@@ -3211,13 +3238,14 @@
       <c r="CF11" s="2"/>
       <c r="CG11" s="2"/>
       <c r="CH11" s="2"/>
+      <c r="CI11" s="2"/>
     </row>
-    <row r="12" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="26"/>
@@ -3318,13 +3346,14 @@
       <c r="CF12" s="2"/>
       <c r="CG12" s="2"/>
       <c r="CH12" s="2"/>
+      <c r="CI12" s="2"/>
     </row>
-    <row r="13" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="26"/>
@@ -3427,13 +3456,14 @@
       <c r="CF13" s="2"/>
       <c r="CG13" s="2"/>
       <c r="CH13" s="2"/>
+      <c r="CI13" s="2"/>
     </row>
-    <row r="14" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="26"/>
@@ -3538,13 +3568,14 @@
       <c r="CF14" s="2"/>
       <c r="CG14" s="2"/>
       <c r="CH14" s="2"/>
+      <c r="CI14" s="2"/>
     </row>
-    <row r="15" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="26"/>
@@ -3651,13 +3682,14 @@
       <c r="CF15" s="2"/>
       <c r="CG15" s="2"/>
       <c r="CH15" s="2"/>
+      <c r="CI15" s="2"/>
     </row>
-    <row r="16" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="26"/>
@@ -3766,13 +3798,14 @@
       <c r="CF16" s="2"/>
       <c r="CG16" s="2"/>
       <c r="CH16" s="2"/>
+      <c r="CI16" s="2"/>
     </row>
-    <row r="17" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="26"/>
@@ -3883,19 +3916,20 @@
       <c r="CF17" s="2"/>
       <c r="CG17" s="2"/>
       <c r="CH17" s="2"/>
+      <c r="CI17" s="2"/>
     </row>
-    <row r="18" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D18" s="30" t="s">
         <v>219</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>224</v>
       </c>
       <c r="E18" s="2">
         <v>2</v>
@@ -4007,19 +4041,20 @@
       <c r="CF18" s="1"/>
       <c r="CG18" s="1"/>
       <c r="CH18" s="1"/>
+      <c r="CI18" s="1"/>
     </row>
-    <row r="19" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="30" t="s">
         <v>217</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>222</v>
       </c>
       <c r="E19" s="2">
         <v>2</v>
@@ -4133,19 +4168,20 @@
       <c r="CF19" s="1"/>
       <c r="CG19" s="1"/>
       <c r="CH19" s="1"/>
+      <c r="CI19" s="1"/>
     </row>
-    <row r="20" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D20" s="30" t="s">
         <v>218</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>223</v>
       </c>
       <c r="E20" s="2">
         <v>2</v>
@@ -4261,19 +4297,20 @@
       <c r="CF20" s="1"/>
       <c r="CG20" s="1"/>
       <c r="CH20" s="1"/>
+      <c r="CI20" s="1"/>
     </row>
-    <row r="21" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E21" s="2">
         <v>2</v>
@@ -4391,19 +4428,20 @@
       <c r="CF21" s="1"/>
       <c r="CG21" s="1"/>
       <c r="CH21" s="1"/>
+      <c r="CI21" s="1"/>
     </row>
-    <row r="22" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E22" s="2">
         <v>2</v>
@@ -4523,19 +4561,20 @@
       <c r="CF22" s="1"/>
       <c r="CG22" s="1"/>
       <c r="CH22" s="1"/>
+      <c r="CI22" s="1"/>
     </row>
-    <row r="23" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E23" s="2">
         <v>2</v>
@@ -4657,19 +4696,20 @@
       <c r="CF23" s="1"/>
       <c r="CG23" s="1"/>
       <c r="CH23" s="1"/>
+      <c r="CI23" s="1"/>
     </row>
-    <row r="24" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E24" s="2">
         <v>2</v>
@@ -4793,19 +4833,20 @@
       <c r="CF24" s="1"/>
       <c r="CG24" s="1"/>
       <c r="CH24" s="1"/>
+      <c r="CI24" s="1"/>
     </row>
-    <row r="25" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E25" s="2">
         <v>2</v>
@@ -4931,19 +4972,20 @@
       <c r="CF25" s="1"/>
       <c r="CG25" s="1"/>
       <c r="CH25" s="1"/>
+      <c r="CI25" s="1"/>
     </row>
-    <row r="26" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E26" s="2">
         <v>2</v>
@@ -5071,19 +5113,20 @@
       <c r="CF26" s="1"/>
       <c r="CG26" s="1"/>
       <c r="CH26" s="1"/>
+      <c r="CI26" s="1"/>
     </row>
-    <row r="27" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
@@ -5213,19 +5256,20 @@
       <c r="CF27" s="1"/>
       <c r="CG27" s="1"/>
       <c r="CH27" s="1"/>
+      <c r="CI27" s="1"/>
     </row>
-    <row r="28" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E28" s="2">
         <v>2</v>
@@ -5357,19 +5401,20 @@
       <c r="CF28" s="1"/>
       <c r="CG28" s="1"/>
       <c r="CH28" s="1"/>
+      <c r="CI28" s="1"/>
     </row>
-    <row r="29" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E29" s="2">
         <v>2</v>
@@ -5503,19 +5548,20 @@
       <c r="CF29" s="1"/>
       <c r="CG29" s="1"/>
       <c r="CH29" s="1"/>
+      <c r="CI29" s="1"/>
     </row>
-    <row r="30" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E30" s="2">
         <v>2</v>
@@ -5651,19 +5697,20 @@
       <c r="CF30" s="1"/>
       <c r="CG30" s="1"/>
       <c r="CH30" s="1"/>
+      <c r="CI30" s="1"/>
     </row>
-    <row r="31" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E31" s="2">
         <v>2</v>
@@ -5801,19 +5848,20 @@
       <c r="CF31" s="1"/>
       <c r="CG31" s="1"/>
       <c r="CH31" s="1"/>
+      <c r="CI31" s="1"/>
     </row>
-    <row r="32" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E32" s="2">
         <v>2</v>
@@ -5953,19 +6001,20 @@
       <c r="CF32" s="1"/>
       <c r="CG32" s="1"/>
       <c r="CH32" s="1"/>
+      <c r="CI32" s="1"/>
     </row>
-    <row r="33" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E33" s="2">
         <v>2</v>
@@ -6107,19 +6156,20 @@
       <c r="CF33" s="1"/>
       <c r="CG33" s="1"/>
       <c r="CH33" s="1"/>
+      <c r="CI33" s="1"/>
     </row>
-    <row r="34" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E34" s="2">
         <v>2</v>
@@ -6263,19 +6313,20 @@
       <c r="CF34" s="1"/>
       <c r="CG34" s="1"/>
       <c r="CH34" s="1"/>
+      <c r="CI34" s="1"/>
     </row>
-    <row r="35" spans="1:86" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:87" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E35" s="2">
         <v>2</v>
@@ -6371,18 +6422,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E36" s="2">
         <v>2</v>
@@ -6530,19 +6581,20 @@
       <c r="CF36" s="1"/>
       <c r="CG36" s="1"/>
       <c r="CH36" s="1"/>
+      <c r="CI36" s="1"/>
     </row>
-    <row r="37" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E37" s="2">
         <v>2</v>
@@ -6692,19 +6744,20 @@
       <c r="CF37" s="1"/>
       <c r="CG37" s="1"/>
       <c r="CH37" s="1"/>
+      <c r="CI37" s="1"/>
     </row>
-    <row r="38" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E38" s="2">
         <v>2</v>
@@ -6856,19 +6909,20 @@
       <c r="CF38" s="1"/>
       <c r="CG38" s="1"/>
       <c r="CH38" s="1"/>
+      <c r="CI38" s="1"/>
     </row>
-    <row r="39" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E39" s="2">
         <v>2</v>
@@ -7022,19 +7076,20 @@
       <c r="CF39" s="1"/>
       <c r="CG39" s="1"/>
       <c r="CH39" s="1"/>
+      <c r="CI39" s="1"/>
     </row>
-    <row r="40" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E40" s="2">
         <v>2</v>
@@ -7190,19 +7245,20 @@
       <c r="CF40" s="1"/>
       <c r="CG40" s="1"/>
       <c r="CH40" s="1"/>
+      <c r="CI40" s="1"/>
     </row>
-    <row r="41" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E41" s="2">
         <v>2</v>
@@ -7360,19 +7416,20 @@
       <c r="CF41" s="1"/>
       <c r="CG41" s="1"/>
       <c r="CH41" s="1"/>
+      <c r="CI41" s="1"/>
     </row>
-    <row r="42" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E42" s="2">
         <v>2</v>
@@ -7532,19 +7589,20 @@
       <c r="CF42" s="1"/>
       <c r="CG42" s="1"/>
       <c r="CH42" s="1"/>
+      <c r="CI42" s="1"/>
     </row>
-    <row r="43" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E43" s="2">
         <v>2</v>
@@ -7706,19 +7764,20 @@
       <c r="CF43" s="1"/>
       <c r="CG43" s="1"/>
       <c r="CH43" s="1"/>
+      <c r="CI43" s="1"/>
     </row>
-    <row r="44" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E44" s="2">
         <v>2</v>
@@ -7882,19 +7941,20 @@
       <c r="CF44" s="1"/>
       <c r="CG44" s="1"/>
       <c r="CH44" s="1"/>
+      <c r="CI44" s="1"/>
     </row>
-    <row r="45" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E45" s="2">
         <v>2</v>
@@ -8060,19 +8120,20 @@
       <c r="CF45" s="1"/>
       <c r="CG45" s="1"/>
       <c r="CH45" s="1"/>
+      <c r="CI45" s="1"/>
     </row>
-    <row r="46" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E46" s="2">
         <v>2</v>
@@ -8240,19 +8301,20 @@
       <c r="CF46" s="1"/>
       <c r="CG46" s="1"/>
       <c r="CH46" s="1"/>
+      <c r="CI46" s="1"/>
     </row>
-    <row r="47" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E47" s="2">
         <v>2</v>
@@ -8422,19 +8484,20 @@
       <c r="CF47" s="1"/>
       <c r="CG47" s="1"/>
       <c r="CH47" s="1"/>
+      <c r="CI47" s="1"/>
     </row>
-    <row r="48" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E48" s="2">
         <v>2</v>
@@ -8606,19 +8669,20 @@
       <c r="CF48" s="1"/>
       <c r="CG48" s="1"/>
       <c r="CH48" s="1"/>
+      <c r="CI48" s="1"/>
     </row>
-    <row r="49" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E49" s="2">
         <v>2</v>
@@ -8792,19 +8856,20 @@
       <c r="CF49" s="1"/>
       <c r="CG49" s="1"/>
       <c r="CH49" s="1"/>
+      <c r="CI49" s="1"/>
     </row>
-    <row r="50" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E50" s="2">
         <v>2</v>
@@ -8980,19 +9045,20 @@
       <c r="CF50" s="1"/>
       <c r="CG50" s="1"/>
       <c r="CH50" s="1"/>
+      <c r="CI50" s="1"/>
     </row>
-    <row r="51" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E51" s="2">
         <v>2</v>
@@ -9170,19 +9236,20 @@
       <c r="CF51" s="1"/>
       <c r="CG51" s="1"/>
       <c r="CH51" s="1"/>
+      <c r="CI51" s="1"/>
     </row>
-    <row r="52" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E52" s="2">
         <v>0</v>
@@ -9362,19 +9429,20 @@
       <c r="CF52" s="1"/>
       <c r="CG52" s="1"/>
       <c r="CH52" s="1"/>
+      <c r="CI52" s="1"/>
     </row>
-    <row r="53" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E53" s="2">
         <v>2</v>
@@ -9556,19 +9624,20 @@
       <c r="CF53" s="1"/>
       <c r="CG53" s="1"/>
       <c r="CH53" s="1"/>
+      <c r="CI53" s="1"/>
     </row>
-    <row r="54" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E54" s="2">
         <v>2</v>
@@ -9752,19 +9821,20 @@
       <c r="CF54" s="1"/>
       <c r="CG54" s="1"/>
       <c r="CH54" s="1"/>
+      <c r="CI54" s="1"/>
     </row>
-    <row r="55" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E55" s="2">
         <v>0</v>
@@ -9950,19 +10020,20 @@
       <c r="CF55" s="1"/>
       <c r="CG55" s="1"/>
       <c r="CH55" s="1"/>
+      <c r="CI55" s="1"/>
     </row>
-    <row r="56" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E56" s="2">
         <v>0</v>
@@ -10150,19 +10221,20 @@
       <c r="CF56" s="1"/>
       <c r="CG56" s="1"/>
       <c r="CH56" s="1"/>
+      <c r="CI56" s="1"/>
     </row>
-    <row r="57" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E57" s="2">
         <v>0</v>
@@ -10352,19 +10424,20 @@
       <c r="CF57" s="1"/>
       <c r="CG57" s="1"/>
       <c r="CH57" s="1"/>
+      <c r="CI57" s="1"/>
     </row>
-    <row r="58" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A58" s="31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E58" s="2">
         <v>0</v>
@@ -10556,19 +10629,20 @@
       <c r="CF58" s="1"/>
       <c r="CG58" s="1"/>
       <c r="CH58" s="1"/>
+      <c r="CI58" s="1"/>
     </row>
-    <row r="59" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A59" s="31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
@@ -10762,19 +10836,20 @@
       <c r="CF59" s="1"/>
       <c r="CG59" s="1"/>
       <c r="CH59" s="1"/>
+      <c r="CI59" s="1"/>
     </row>
-    <row r="60" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A60" s="31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D60" s="32" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E60" s="2">
         <v>0</v>
@@ -10970,19 +11045,20 @@
       <c r="CF60" s="1"/>
       <c r="CG60" s="1"/>
       <c r="CH60" s="1"/>
+      <c r="CI60" s="1"/>
     </row>
-    <row r="61" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E61" s="2">
         <v>0</v>
@@ -11180,19 +11256,20 @@
       <c r="CF61" s="1"/>
       <c r="CG61" s="1"/>
       <c r="CH61" s="1"/>
+      <c r="CI61" s="1"/>
     </row>
-    <row r="62" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E62" s="2">
         <v>0</v>
@@ -11392,19 +11469,20 @@
       <c r="CF62" s="1"/>
       <c r="CG62" s="1"/>
       <c r="CH62" s="1"/>
+      <c r="CI62" s="1"/>
     </row>
-    <row r="63" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A63" s="31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D63" s="32" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E63" s="2">
         <v>0</v>
@@ -11606,19 +11684,20 @@
       <c r="CF63" s="1"/>
       <c r="CG63" s="1"/>
       <c r="CH63" s="1"/>
+      <c r="CI63" s="1"/>
     </row>
-    <row r="64" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E64" s="2">
         <v>0</v>
@@ -11822,19 +11901,20 @@
       <c r="CF64" s="1"/>
       <c r="CG64" s="1"/>
       <c r="CH64" s="1"/>
+      <c r="CI64" s="1"/>
     </row>
-    <row r="65" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A65" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D65" s="32" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E65" s="2">
         <v>0</v>
@@ -12040,19 +12120,20 @@
       <c r="CF65" s="1"/>
       <c r="CG65" s="1"/>
       <c r="CH65" s="1"/>
+      <c r="CI65" s="1"/>
     </row>
-    <row r="66" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D66" s="34" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E66" s="2">
         <v>2</v>
@@ -12260,19 +12341,20 @@
       <c r="CF66" s="1"/>
       <c r="CG66" s="1"/>
       <c r="CH66" s="1"/>
+      <c r="CI66" s="1"/>
     </row>
-    <row r="67" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D67" s="34" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E67" s="2">
         <v>2</v>
@@ -12482,19 +12564,20 @@
       <c r="CF67" s="1"/>
       <c r="CG67" s="1"/>
       <c r="CH67" s="1"/>
+      <c r="CI67" s="1"/>
     </row>
-    <row r="68" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E68" s="2">
         <v>2</v>
@@ -12706,19 +12789,20 @@
       <c r="CF68" s="1"/>
       <c r="CG68" s="1"/>
       <c r="CH68" s="1"/>
+      <c r="CI68" s="1"/>
     </row>
-    <row r="69" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D69" s="34" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E69" s="2">
         <v>2</v>
@@ -12932,19 +13016,20 @@
       <c r="CF69" s="1"/>
       <c r="CG69" s="1"/>
       <c r="CH69" s="1"/>
+      <c r="CI69" s="1"/>
     </row>
-    <row r="70" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D70" s="34" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E70" s="2">
         <v>2</v>
@@ -13160,19 +13245,20 @@
       <c r="CF70" s="1"/>
       <c r="CG70" s="1"/>
       <c r="CH70" s="1"/>
+      <c r="CI70" s="1"/>
     </row>
-    <row r="71" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E71" s="2">
         <v>2</v>
@@ -13390,19 +13476,20 @@
       <c r="CF71" s="1"/>
       <c r="CG71" s="1"/>
       <c r="CH71" s="1"/>
+      <c r="CI71" s="1"/>
     </row>
-    <row r="72" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D72" s="34" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E72" s="2">
         <v>2</v>
@@ -13622,19 +13709,20 @@
       <c r="CF72" s="1"/>
       <c r="CG72" s="1"/>
       <c r="CH72" s="1"/>
+      <c r="CI72" s="1"/>
     </row>
-    <row r="73" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D73" s="34" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E73" s="2">
         <v>0</v>
@@ -13856,19 +13944,20 @@
       <c r="CF73" s="1"/>
       <c r="CG73" s="1"/>
       <c r="CH73" s="1"/>
+      <c r="CI73" s="1"/>
     </row>
-    <row r="74" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D74" s="34" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E74" s="2">
         <v>0</v>
@@ -14092,19 +14181,20 @@
       <c r="CF74" s="1"/>
       <c r="CG74" s="1"/>
       <c r="CH74" s="1"/>
+      <c r="CI74" s="1"/>
     </row>
-    <row r="75" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D75" s="34" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E75" s="2">
         <v>0</v>
@@ -14330,19 +14420,20 @@
       <c r="CF75" s="1"/>
       <c r="CG75" s="1"/>
       <c r="CH75" s="1"/>
+      <c r="CI75" s="1"/>
     </row>
-    <row r="76" spans="1:86" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:87" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E76" s="2">
         <v>0</v>
@@ -14570,19 +14661,20 @@
       <c r="CF76" s="1"/>
       <c r="CG76" s="1"/>
       <c r="CH76" s="1"/>
+      <c r="CI76" s="1"/>
     </row>
-    <row r="77" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D77" s="34" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E77" s="2">
         <v>0</v>
@@ -14812,19 +14904,20 @@
       <c r="CF77" s="1"/>
       <c r="CG77" s="1"/>
       <c r="CH77" s="1"/>
+      <c r="CI77" s="1"/>
     </row>
-    <row r="78" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D78" s="34" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E78" s="2">
         <v>0</v>
@@ -15056,19 +15149,20 @@
       <c r="CF78" s="1"/>
       <c r="CG78" s="1"/>
       <c r="CH78" s="1"/>
+      <c r="CI78" s="1"/>
     </row>
-    <row r="79" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D79" s="34" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E79" s="2">
         <v>0</v>
@@ -15302,19 +15396,20 @@
       <c r="CF79" s="1"/>
       <c r="CG79" s="1"/>
       <c r="CH79" s="1"/>
+      <c r="CI79" s="1"/>
     </row>
-    <row r="80" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D80" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E80" s="2">
         <v>0</v>
@@ -15550,19 +15645,20 @@
       <c r="CF80" s="1"/>
       <c r="CG80" s="1"/>
       <c r="CH80" s="1"/>
+      <c r="CI80" s="1"/>
     </row>
-    <row r="81" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D81" s="34" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E81" s="2">
         <v>0</v>
@@ -15800,19 +15896,20 @@
       <c r="CF81" s="1"/>
       <c r="CG81" s="1"/>
       <c r="CH81" s="1"/>
+      <c r="CI81" s="1"/>
     </row>
-    <row r="82" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="33" t="s">
-        <v>126</v>
+        <v>225</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="D82" s="34" t="s">
-        <v>190</v>
+        <v>226</v>
       </c>
       <c r="E82" s="2">
         <v>0</v>
@@ -15965,40 +16062,40 @@
         <v>1</v>
       </c>
       <c r="BC82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO82" s="1">
         <v>0</v>
@@ -16052,19 +16149,20 @@
       <c r="CF82" s="1"/>
       <c r="CG82" s="1"/>
       <c r="CH82" s="1"/>
+      <c r="CI82" s="1"/>
     </row>
-    <row r="83" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="33" t="s">
-        <v>127</v>
+        <v>228</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>60</v>
+        <v>229</v>
       </c>
       <c r="D83" s="34" t="s">
-        <v>191</v>
+        <v>230</v>
       </c>
       <c r="E83" s="2">
         <v>0</v>
@@ -16217,40 +16315,40 @@
         <v>1</v>
       </c>
       <c r="BC83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO83" s="1">
         <v>0</v>
@@ -16306,19 +16404,20 @@
       <c r="CF83" s="1"/>
       <c r="CG83" s="1"/>
       <c r="CH83" s="1"/>
+      <c r="CI83" s="1"/>
     </row>
-    <row r="84" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A84" s="33" t="s">
-        <v>128</v>
+        <v>227</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>61</v>
+        <v>223</v>
       </c>
       <c r="D84" s="34" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E84" s="2">
         <v>0</v>
@@ -16462,7 +16561,7 @@
         <v>0</v>
       </c>
       <c r="AZ84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA84" s="1">
         <v>1</v>
@@ -16471,40 +16570,40 @@
         <v>1</v>
       </c>
       <c r="BC84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO84" s="1">
         <v>0</v>
@@ -16562,34 +16661,35 @@
       </c>
       <c r="CG84" s="1"/>
       <c r="CH84" s="1"/>
+      <c r="CI84" s="1"/>
     </row>
-    <row r="85" spans="1:86" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:87" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="33" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D85" s="34" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E85" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F85" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G85" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H85" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I85" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J85" s="2">
         <v>2</v>
@@ -16616,31 +16716,31 @@
         <v>0</v>
       </c>
       <c r="R85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA85" s="1">
         <v>1</v>
@@ -16763,13 +16863,13 @@
         <v>0</v>
       </c>
       <c r="BO85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR85" s="1">
         <v>0</v>
@@ -16787,7 +16887,7 @@
         <v>0</v>
       </c>
       <c r="BW85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX85" s="1">
         <v>0</v>
@@ -16820,19 +16920,20 @@
         <v>3</v>
       </c>
       <c r="CH85" s="1"/>
+      <c r="CI85" s="1"/>
     </row>
-    <row r="86" spans="1:86" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="B86" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C86" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="D86" s="37" t="s">
-        <v>194</v>
+    <row r="86" spans="1:87" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D86" s="34" t="s">
+        <v>188</v>
       </c>
       <c r="E86" s="2">
         <v>2</v>
@@ -16850,7 +16951,7 @@
         <v>2</v>
       </c>
       <c r="J86" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K86" s="1">
         <v>0</v>
@@ -16868,7 +16969,7 @@
         <v>0</v>
       </c>
       <c r="P86" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q86" s="2">
         <v>0</v>
@@ -16901,7 +17002,7 @@
         <v>1</v>
       </c>
       <c r="AA86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB86" s="1">
         <v>0</v>
@@ -16916,10 +17017,10 @@
         <v>0</v>
       </c>
       <c r="AF86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH86" s="1">
         <v>0</v>
@@ -16979,10 +17080,10 @@
         <v>0</v>
       </c>
       <c r="BA86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC86" s="1">
         <v>0</v>
@@ -17018,16 +17119,16 @@
         <v>0</v>
       </c>
       <c r="BN86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO86" s="1">
         <v>1</v>
       </c>
       <c r="BP86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR86" s="1">
         <v>0</v>
@@ -17045,7 +17146,7 @@
         <v>0</v>
       </c>
       <c r="BW86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX86" s="1">
         <v>0</v>
@@ -17069,10 +17170,10 @@
         <v>0</v>
       </c>
       <c r="CE86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG86" s="1">
         <v>0</v>
@@ -17080,10 +17181,274 @@
       <c r="CH86" s="1">
         <v>3</v>
       </c>
+      <c r="CI86" s="1"/>
+    </row>
+    <row r="87" spans="1:87" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B87" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C87" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D87" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="E87" s="2">
+        <v>2</v>
+      </c>
+      <c r="F87" s="2">
+        <v>2</v>
+      </c>
+      <c r="G87" s="2">
+        <v>2</v>
+      </c>
+      <c r="H87" s="2">
+        <v>1</v>
+      </c>
+      <c r="I87" s="2">
+        <v>2</v>
+      </c>
+      <c r="J87" s="2">
+        <v>0</v>
+      </c>
+      <c r="K87" s="1">
+        <v>0</v>
+      </c>
+      <c r="L87" s="2">
+        <v>0</v>
+      </c>
+      <c r="M87" s="2">
+        <v>0</v>
+      </c>
+      <c r="N87" s="2">
+        <v>0</v>
+      </c>
+      <c r="O87" s="2">
+        <v>0</v>
+      </c>
+      <c r="P87" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q87" s="2">
+        <v>0</v>
+      </c>
+      <c r="R87" s="1">
+        <v>1</v>
+      </c>
+      <c r="S87" s="1">
+        <v>1</v>
+      </c>
+      <c r="T87" s="1">
+        <v>1</v>
+      </c>
+      <c r="U87" s="1">
+        <v>1</v>
+      </c>
+      <c r="V87" s="1">
+        <v>1</v>
+      </c>
+      <c r="W87" s="1">
+        <v>1</v>
+      </c>
+      <c r="X87" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y87" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z87" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF87" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG87" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN87" s="1">
+        <v>1</v>
+      </c>
+      <c r="BO87" s="1">
+        <v>1</v>
+      </c>
+      <c r="BP87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY87" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ87" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA87" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB87" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC87" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD87" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE87" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF87" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG87" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH87" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI87" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:CH4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A1:CH86">
+  <autoFilter ref="A4:CI4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A1:CI87">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
qlang: added "$deduplicate;" instruction
Changes to be committed:
	modified:   qplib/data/symbols.csv
	modified:   qplib/data/symbols.xlsx
	modified:   qplib/qlang.py
</commit_message>
<xml_diff>
--- a/qplib/data/symbols.xlsx
+++ b/qplib/data/symbols.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinVölkl\Desktop\qplib_dev\qplib\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C59825-D170-42B7-BFDA-F97F39616348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E60AF1-135C-4706-A1AD-C5801E9FF9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$CJ$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$CK$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="235">
   <si>
     <t>"%%"</t>
   </si>
@@ -754,6 +754,15 @@
   </si>
   <si>
     <t>modify_scope</t>
+  </si>
+  <si>
+    <t>DEDUPLICATE</t>
+  </si>
+  <si>
+    <t>"deduplicate;"</t>
+  </si>
+  <si>
+    <t>deduplicate by appending consecutive numbers. Tranforms values to str.</t>
   </si>
 </sst>
 </file>
@@ -1476,20 +1485,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CJ88"/>
+  <dimension ref="A1:CK89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="S58" sqref="S58"/>
+      <selection pane="bottomRight" activeCell="P55" sqref="P55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="32.140625" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -1525,36 +1534,39 @@
     <col min="44" max="44" width="10.5703125" style="38" customWidth="1"/>
     <col min="45" max="45" width="11.28515625" style="38" customWidth="1"/>
     <col min="46" max="46" width="13" style="38" customWidth="1"/>
-    <col min="47" max="52" width="13.7109375" style="38" customWidth="1"/>
+    <col min="47" max="50" width="13.7109375" style="38" customWidth="1"/>
+    <col min="51" max="51" width="18" style="38" customWidth="1"/>
+    <col min="52" max="52" width="16" style="38" customWidth="1"/>
     <col min="53" max="53" width="18.85546875" style="38" customWidth="1"/>
     <col min="54" max="54" width="11.28515625" style="38" customWidth="1"/>
     <col min="55" max="55" width="17" style="38" customWidth="1"/>
     <col min="56" max="56" width="16.85546875" style="38" customWidth="1"/>
-    <col min="57" max="66" width="12.42578125" style="38" customWidth="1"/>
-    <col min="67" max="67" width="14.28515625" style="38" customWidth="1"/>
-    <col min="68" max="68" width="26.7109375" style="38" customWidth="1"/>
-    <col min="69" max="69" width="26.140625" style="38" customWidth="1"/>
-    <col min="70" max="70" width="22.28515625" style="38" customWidth="1"/>
-    <col min="71" max="71" width="24.5703125" style="38" customWidth="1"/>
-    <col min="72" max="72" width="25.140625" style="38" customWidth="1"/>
-    <col min="73" max="73" width="27.85546875" style="38" customWidth="1"/>
-    <col min="74" max="74" width="19.42578125" style="38" customWidth="1"/>
-    <col min="75" max="75" width="27" style="38" customWidth="1"/>
-    <col min="76" max="76" width="19.85546875" style="38" customWidth="1"/>
-    <col min="77" max="77" width="30.7109375" style="38" customWidth="1"/>
-    <col min="78" max="78" width="16" style="38" customWidth="1"/>
-    <col min="79" max="79" width="22.7109375" style="38" customWidth="1"/>
-    <col min="80" max="80" width="17.28515625" style="38" customWidth="1"/>
-    <col min="81" max="81" width="15.7109375" style="38" customWidth="1"/>
-    <col min="82" max="82" width="16.28515625" style="38" customWidth="1"/>
-    <col min="83" max="83" width="18.5703125" style="38" customWidth="1"/>
-    <col min="84" max="85" width="13.7109375" style="38" customWidth="1"/>
-    <col min="86" max="86" width="15.7109375" style="38" customWidth="1"/>
-    <col min="87" max="87" width="22.42578125" style="38" customWidth="1"/>
-    <col min="88" max="88" width="17.140625" style="38" customWidth="1"/>
+    <col min="57" max="57" width="25.42578125" style="38" customWidth="1"/>
+    <col min="58" max="67" width="12.42578125" style="38" customWidth="1"/>
+    <col min="68" max="68" width="14.28515625" style="38" customWidth="1"/>
+    <col min="69" max="69" width="26.7109375" style="38" customWidth="1"/>
+    <col min="70" max="70" width="26.140625" style="38" customWidth="1"/>
+    <col min="71" max="71" width="22.28515625" style="38" customWidth="1"/>
+    <col min="72" max="72" width="24.5703125" style="38" customWidth="1"/>
+    <col min="73" max="73" width="25.140625" style="38" customWidth="1"/>
+    <col min="74" max="74" width="27.85546875" style="38" customWidth="1"/>
+    <col min="75" max="75" width="19.42578125" style="38" customWidth="1"/>
+    <col min="76" max="76" width="27" style="38" customWidth="1"/>
+    <col min="77" max="77" width="19.85546875" style="38" customWidth="1"/>
+    <col min="78" max="78" width="30.7109375" style="38" customWidth="1"/>
+    <col min="79" max="79" width="16" style="38" customWidth="1"/>
+    <col min="80" max="80" width="22.7109375" style="38" customWidth="1"/>
+    <col min="81" max="81" width="17.28515625" style="38" customWidth="1"/>
+    <col min="82" max="82" width="15.7109375" style="38" customWidth="1"/>
+    <col min="83" max="83" width="16.28515625" style="38" customWidth="1"/>
+    <col min="84" max="84" width="18.5703125" style="38" customWidth="1"/>
+    <col min="85" max="86" width="13.7109375" style="38" customWidth="1"/>
+    <col min="87" max="87" width="15.7109375" style="38" customWidth="1"/>
+    <col min="88" max="88" width="22.42578125" style="38" customWidth="1"/>
+    <col min="89" max="89" width="17.140625" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:89" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>190</v>
@@ -1722,103 +1734,106 @@
         <v>95</v>
       </c>
       <c r="BE1" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="BF1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="BF1" s="15" t="s">
+      <c r="BG1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="BG1" s="15" t="s">
+      <c r="BH1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="BH1" s="15" t="s">
+      <c r="BI1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="BI1" s="15" t="s">
+      <c r="BJ1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="BJ1" s="15" t="s">
+      <c r="BK1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="BK1" s="15" t="s">
+      <c r="BL1" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="BL1" s="15" t="s">
+      <c r="BM1" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="BM1" s="15" t="s">
+      <c r="BN1" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="BN1" s="15" t="s">
+      <c r="BO1" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="BO1" s="16" t="s">
+      <c r="BP1" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="BP1" s="16" t="s">
+      <c r="BQ1" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="BQ1" s="16" t="s">
+      <c r="BR1" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="BR1" s="16" t="s">
+      <c r="BS1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="BS1" s="16" t="s">
+      <c r="BT1" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="BT1" s="16" t="s">
+      <c r="BU1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="BU1" s="16" t="s">
+      <c r="BV1" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="BV1" s="16" t="s">
+      <c r="BW1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="BW1" s="16" t="s">
+      <c r="BX1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="BX1" s="16" t="s">
+      <c r="BY1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="BY1" s="16" t="s">
+      <c r="BZ1" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="BZ1" s="16" t="s">
+      <c r="CA1" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="CA1" s="16" t="s">
+      <c r="CB1" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="CB1" s="16" t="s">
+      <c r="CC1" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="CC1" s="16" t="s">
+      <c r="CD1" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="CD1" s="16" t="s">
+      <c r="CE1" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="CE1" s="16" t="s">
+      <c r="CF1" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="CF1" s="16" t="s">
+      <c r="CG1" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="CG1" s="16" t="s">
+      <c r="CH1" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="CH1" s="16" t="s">
+      <c r="CI1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="CI1" s="16" t="s">
+      <c r="CJ1" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="CJ1" s="16" t="s">
+      <c r="CK1" s="16" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:88" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:89" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>190</v>
       </c>
@@ -2017,8 +2032,8 @@
       <c r="BN2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BO2" s="5" t="s">
-        <v>64</v>
+      <c r="BO2" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="BP2" s="5" t="s">
         <v>64</v>
@@ -2083,8 +2098,11 @@
       <c r="CJ2" s="5" t="s">
         <v>64</v>
       </c>
+      <c r="CK2" s="5" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="3" spans="1:88" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:89" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>196</v>
       </c>
@@ -2222,103 +2240,106 @@
         <v>30</v>
       </c>
       <c r="BE3" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="BF3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="BF3" s="4" t="s">
+      <c r="BG3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="BG3" s="4" t="s">
+      <c r="BH3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="BH3" s="4" t="s">
+      <c r="BI3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="BI3" s="4" t="s">
+      <c r="BJ3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="BJ3" s="4" t="s">
+      <c r="BK3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="BK3" s="4" t="s">
+      <c r="BL3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="BL3" s="4" t="s">
+      <c r="BM3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="BM3" s="4" t="s">
+      <c r="BN3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BN3" s="4" t="s">
+      <c r="BO3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="BO3" s="5" t="s">
+      <c r="BP3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="BP3" s="5" t="s">
+      <c r="BQ3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="BQ3" s="5" t="s">
+      <c r="BR3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BR3" s="5" t="s">
+      <c r="BS3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="BS3" s="5" t="s">
+      <c r="BT3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="BT3" s="5" t="s">
+      <c r="BU3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="BU3" s="5" t="s">
+      <c r="BV3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="BV3" s="5" t="s">
+      <c r="BW3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="BW3" s="5" t="s">
+      <c r="BX3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="BX3" s="5" t="s">
+      <c r="BY3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="BY3" s="5" t="s">
+      <c r="BZ3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="BZ3" s="5" t="s">
+      <c r="CA3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="CA3" s="5" t="s">
+      <c r="CB3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="CB3" s="5" t="s">
+      <c r="CC3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="CC3" s="5" t="s">
+      <c r="CD3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="CD3" s="5" t="s">
+      <c r="CE3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="CE3" s="5" t="s">
+      <c r="CF3" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="CF3" s="5" t="s">
+      <c r="CG3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="CG3" s="5" t="s">
+      <c r="CH3" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="CH3" s="5" t="s">
+      <c r="CI3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="CI3" s="5" t="s">
+      <c r="CJ3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="CJ3" s="5" t="s">
+      <c r="CK3" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:88" s="23" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:89" s="23" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>191</v>
       </c>
@@ -2456,103 +2477,106 @@
         <v>157</v>
       </c>
       <c r="BE4" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="BF4" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="BF4" s="21" t="s">
+      <c r="BG4" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="BG4" s="21" t="s">
+      <c r="BH4" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="BH4" s="21" t="s">
+      <c r="BI4" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="BI4" s="21" t="s">
+      <c r="BJ4" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="BJ4" s="21" t="s">
+      <c r="BK4" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="BK4" s="21" t="s">
+      <c r="BL4" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="BL4" s="21" t="s">
+      <c r="BM4" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="BM4" s="21" t="s">
+      <c r="BN4" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="BN4" s="21" t="s">
+      <c r="BO4" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="BO4" s="22" t="s">
+      <c r="BP4" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="BP4" s="22" t="s">
+      <c r="BQ4" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="BQ4" s="22" t="s">
+      <c r="BR4" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="BR4" s="22" t="s">
+      <c r="BS4" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="BS4" s="22" t="s">
+      <c r="BT4" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="BT4" s="22" t="s">
+      <c r="BU4" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="BU4" s="22" t="s">
+      <c r="BV4" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="BV4" s="22" t="s">
+      <c r="BW4" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="BW4" s="22" t="s">
+      <c r="BX4" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="BX4" s="22" t="s">
+      <c r="BY4" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="BY4" s="22" t="s">
+      <c r="BZ4" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="BZ4" s="22" t="s">
+      <c r="CA4" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="CA4" s="22" t="s">
+      <c r="CB4" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="CB4" s="22" t="s">
+      <c r="CC4" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="CC4" s="22" t="s">
+      <c r="CD4" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="CD4" s="22" t="s">
+      <c r="CE4" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="CE4" s="22" t="s">
+      <c r="CF4" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="CF4" s="22" t="s">
+      <c r="CG4" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="CG4" s="22" t="s">
+      <c r="CH4" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="CH4" s="22" t="s">
+      <c r="CI4" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="CI4" s="22" t="s">
+      <c r="CJ4" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="CJ4" s="22" t="s">
+      <c r="CK4" s="22" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>193</v>
       </c>
@@ -2646,8 +2670,9 @@
       <c r="CH5" s="2"/>
       <c r="CI5" s="2"/>
       <c r="CJ5" s="2"/>
+      <c r="CK5" s="2"/>
     </row>
-    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>221</v>
       </c>
@@ -2743,8 +2768,9 @@
       <c r="CH6" s="2"/>
       <c r="CI6" s="2"/>
       <c r="CJ6" s="2"/>
+      <c r="CK6" s="2"/>
     </row>
-    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>194</v>
       </c>
@@ -2842,8 +2868,9 @@
       <c r="CH7" s="2"/>
       <c r="CI7" s="2"/>
       <c r="CJ7" s="2"/>
+      <c r="CK7" s="2"/>
     </row>
-    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>200</v>
       </c>
@@ -2943,8 +2970,9 @@
       <c r="CH8" s="2"/>
       <c r="CI8" s="2"/>
       <c r="CJ8" s="2"/>
+      <c r="CK8" s="2"/>
     </row>
-    <row r="9" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>195</v>
       </c>
@@ -3046,8 +3074,9 @@
       <c r="CH9" s="2"/>
       <c r="CI9" s="2"/>
       <c r="CJ9" s="2"/>
+      <c r="CK9" s="2"/>
     </row>
-    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>199</v>
       </c>
@@ -3151,8 +3180,9 @@
       <c r="CH10" s="2"/>
       <c r="CI10" s="2"/>
       <c r="CJ10" s="2"/>
+      <c r="CK10" s="2"/>
     </row>
-    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>231</v>
       </c>
@@ -3258,8 +3288,9 @@
       <c r="CH11" s="2"/>
       <c r="CI11" s="2"/>
       <c r="CJ11" s="2"/>
+      <c r="CK11" s="2"/>
     </row>
-    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>192</v>
       </c>
@@ -3367,8 +3398,9 @@
       <c r="CH12" s="2"/>
       <c r="CI12" s="2"/>
       <c r="CJ12" s="2"/>
+      <c r="CK12" s="2"/>
     </row>
-    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>197</v>
       </c>
@@ -3478,8 +3510,9 @@
       <c r="CH13" s="2"/>
       <c r="CI13" s="2"/>
       <c r="CJ13" s="2"/>
+      <c r="CK13" s="2"/>
     </row>
-    <row r="14" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>201</v>
       </c>
@@ -3591,8 +3624,9 @@
       <c r="CH14" s="2"/>
       <c r="CI14" s="2"/>
       <c r="CJ14" s="2"/>
+      <c r="CK14" s="2"/>
     </row>
-    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>202</v>
       </c>
@@ -3706,8 +3740,9 @@
       <c r="CH15" s="2"/>
       <c r="CI15" s="2"/>
       <c r="CJ15" s="2"/>
+      <c r="CK15" s="2"/>
     </row>
-    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>203</v>
       </c>
@@ -3823,8 +3858,9 @@
       <c r="CH16" s="2"/>
       <c r="CI16" s="2"/>
       <c r="CJ16" s="2"/>
+      <c r="CK16" s="2"/>
     </row>
-    <row r="17" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>204</v>
       </c>
@@ -3942,8 +3978,9 @@
       <c r="CH17" s="2"/>
       <c r="CI17" s="2"/>
       <c r="CJ17" s="2"/>
+      <c r="CK17" s="2"/>
     </row>
-    <row r="18" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>205</v>
       </c>
@@ -4063,8 +4100,9 @@
       <c r="CH18" s="2"/>
       <c r="CI18" s="2"/>
       <c r="CJ18" s="2"/>
+      <c r="CK18" s="2"/>
     </row>
-    <row r="19" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>211</v>
       </c>
@@ -4191,8 +4229,9 @@
       <c r="CH19" s="1"/>
       <c r="CI19" s="1"/>
       <c r="CJ19" s="1"/>
+      <c r="CK19" s="1"/>
     </row>
-    <row r="20" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>212</v>
       </c>
@@ -4321,8 +4360,9 @@
       <c r="CH20" s="1"/>
       <c r="CI20" s="1"/>
       <c r="CJ20" s="1"/>
+      <c r="CK20" s="1"/>
     </row>
-    <row r="21" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>213</v>
       </c>
@@ -4453,8 +4493,9 @@
       <c r="CH21" s="1"/>
       <c r="CI21" s="1"/>
       <c r="CJ21" s="1"/>
+      <c r="CK21" s="1"/>
     </row>
-    <row r="22" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>65</v>
       </c>
@@ -4587,8 +4628,9 @@
       <c r="CH22" s="1"/>
       <c r="CI22" s="1"/>
       <c r="CJ22" s="1"/>
+      <c r="CK22" s="1"/>
     </row>
-    <row r="23" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>66</v>
       </c>
@@ -4723,8 +4765,9 @@
       <c r="CH23" s="1"/>
       <c r="CI23" s="1"/>
       <c r="CJ23" s="1"/>
+      <c r="CK23" s="1"/>
     </row>
-    <row r="24" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>67</v>
       </c>
@@ -4861,8 +4904,9 @@
       <c r="CH24" s="1"/>
       <c r="CI24" s="1"/>
       <c r="CJ24" s="1"/>
+      <c r="CK24" s="1"/>
     </row>
-    <row r="25" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>68</v>
       </c>
@@ -5001,8 +5045,9 @@
       <c r="CH25" s="1"/>
       <c r="CI25" s="1"/>
       <c r="CJ25" s="1"/>
+      <c r="CK25" s="1"/>
     </row>
-    <row r="26" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>69</v>
       </c>
@@ -5143,8 +5188,9 @@
       <c r="CH26" s="1"/>
       <c r="CI26" s="1"/>
       <c r="CJ26" s="1"/>
+      <c r="CK26" s="1"/>
     </row>
-    <row r="27" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
         <v>70</v>
       </c>
@@ -5287,8 +5333,9 @@
       <c r="CH27" s="1"/>
       <c r="CI27" s="1"/>
       <c r="CJ27" s="1"/>
+      <c r="CK27" s="1"/>
     </row>
-    <row r="28" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>71</v>
       </c>
@@ -5433,8 +5480,9 @@
       <c r="CH28" s="1"/>
       <c r="CI28" s="1"/>
       <c r="CJ28" s="1"/>
+      <c r="CK28" s="1"/>
     </row>
-    <row r="29" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>72</v>
       </c>
@@ -5581,8 +5629,9 @@
       <c r="CH29" s="1"/>
       <c r="CI29" s="1"/>
       <c r="CJ29" s="1"/>
+      <c r="CK29" s="1"/>
     </row>
-    <row r="30" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>73</v>
       </c>
@@ -5731,8 +5780,9 @@
       <c r="CH30" s="1"/>
       <c r="CI30" s="1"/>
       <c r="CJ30" s="1"/>
+      <c r="CK30" s="1"/>
     </row>
-    <row r="31" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>74</v>
       </c>
@@ -5883,8 +5933,9 @@
       <c r="CH31" s="1"/>
       <c r="CI31" s="1"/>
       <c r="CJ31" s="1"/>
+      <c r="CK31" s="1"/>
     </row>
-    <row r="32" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>75</v>
       </c>
@@ -6037,8 +6088,9 @@
       <c r="CH32" s="1"/>
       <c r="CI32" s="1"/>
       <c r="CJ32" s="1"/>
+      <c r="CK32" s="1"/>
     </row>
-    <row r="33" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>76</v>
       </c>
@@ -6193,8 +6245,9 @@
       <c r="CH33" s="1"/>
       <c r="CI33" s="1"/>
       <c r="CJ33" s="1"/>
+      <c r="CK33" s="1"/>
     </row>
-    <row r="34" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>77</v>
       </c>
@@ -6351,8 +6404,9 @@
       <c r="CH34" s="1"/>
       <c r="CI34" s="1"/>
       <c r="CJ34" s="1"/>
+      <c r="CK34" s="1"/>
     </row>
-    <row r="35" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>206</v>
       </c>
@@ -6511,8 +6565,9 @@
       <c r="CH35" s="1"/>
       <c r="CI35" s="1"/>
       <c r="CJ35" s="1"/>
+      <c r="CK35" s="1"/>
     </row>
-    <row r="36" spans="1:88" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:89" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>208</v>
       </c>
@@ -6622,7 +6677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>78</v>
       </c>
@@ -6785,8 +6840,9 @@
       <c r="CH37" s="1"/>
       <c r="CI37" s="1"/>
       <c r="CJ37" s="1"/>
+      <c r="CK37" s="1"/>
     </row>
-    <row r="38" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>79</v>
       </c>
@@ -6951,8 +7007,9 @@
       <c r="CH38" s="1"/>
       <c r="CI38" s="1"/>
       <c r="CJ38" s="1"/>
+      <c r="CK38" s="1"/>
     </row>
-    <row r="39" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>80</v>
       </c>
@@ -7119,8 +7176,9 @@
       <c r="CH39" s="1"/>
       <c r="CI39" s="1"/>
       <c r="CJ39" s="1"/>
+      <c r="CK39" s="1"/>
     </row>
-    <row r="40" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>81</v>
       </c>
@@ -7289,8 +7347,9 @@
       <c r="CH40" s="1"/>
       <c r="CI40" s="1"/>
       <c r="CJ40" s="1"/>
+      <c r="CK40" s="1"/>
     </row>
-    <row r="41" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>82</v>
       </c>
@@ -7461,8 +7520,9 @@
       <c r="CH41" s="1"/>
       <c r="CI41" s="1"/>
       <c r="CJ41" s="1"/>
+      <c r="CK41" s="1"/>
     </row>
-    <row r="42" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>83</v>
       </c>
@@ -7635,8 +7695,9 @@
       <c r="CH42" s="1"/>
       <c r="CI42" s="1"/>
       <c r="CJ42" s="1"/>
+      <c r="CK42" s="1"/>
     </row>
-    <row r="43" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>84</v>
       </c>
@@ -7811,8 +7872,9 @@
       <c r="CH43" s="1"/>
       <c r="CI43" s="1"/>
       <c r="CJ43" s="1"/>
+      <c r="CK43" s="1"/>
     </row>
-    <row r="44" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>85</v>
       </c>
@@ -7989,8 +8051,9 @@
       <c r="CH44" s="1"/>
       <c r="CI44" s="1"/>
       <c r="CJ44" s="1"/>
+      <c r="CK44" s="1"/>
     </row>
-    <row r="45" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>86</v>
       </c>
@@ -8169,8 +8232,9 @@
       <c r="CH45" s="1"/>
       <c r="CI45" s="1"/>
       <c r="CJ45" s="1"/>
+      <c r="CK45" s="1"/>
     </row>
-    <row r="46" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
         <v>87</v>
       </c>
@@ -8351,8 +8415,9 @@
       <c r="CH46" s="1"/>
       <c r="CI46" s="1"/>
       <c r="CJ46" s="1"/>
+      <c r="CK46" s="1"/>
     </row>
-    <row r="47" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
         <v>88</v>
       </c>
@@ -8535,8 +8600,9 @@
       <c r="CH47" s="1"/>
       <c r="CI47" s="1"/>
       <c r="CJ47" s="1"/>
+      <c r="CK47" s="1"/>
     </row>
-    <row r="48" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
         <v>89</v>
       </c>
@@ -8721,8 +8787,9 @@
       <c r="CH48" s="1"/>
       <c r="CI48" s="1"/>
       <c r="CJ48" s="1"/>
+      <c r="CK48" s="1"/>
     </row>
-    <row r="49" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
         <v>90</v>
       </c>
@@ -8909,8 +8976,9 @@
       <c r="CH49" s="1"/>
       <c r="CI49" s="1"/>
       <c r="CJ49" s="1"/>
+      <c r="CK49" s="1"/>
     </row>
-    <row r="50" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>91</v>
       </c>
@@ -9099,8 +9167,9 @@
       <c r="CH50" s="1"/>
       <c r="CI50" s="1"/>
       <c r="CJ50" s="1"/>
+      <c r="CK50" s="1"/>
     </row>
-    <row r="51" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
         <v>92</v>
       </c>
@@ -9291,8 +9360,9 @@
       <c r="CH51" s="1"/>
       <c r="CI51" s="1"/>
       <c r="CJ51" s="1"/>
+      <c r="CK51" s="1"/>
     </row>
-    <row r="52" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
         <v>93</v>
       </c>
@@ -9485,8 +9555,9 @@
       <c r="CH52" s="1"/>
       <c r="CI52" s="1"/>
       <c r="CJ52" s="1"/>
+      <c r="CK52" s="1"/>
     </row>
-    <row r="53" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
         <v>94</v>
       </c>
@@ -9681,8 +9752,9 @@
       <c r="CH53" s="1"/>
       <c r="CI53" s="1"/>
       <c r="CJ53" s="1"/>
+      <c r="CK53" s="1"/>
     </row>
-    <row r="54" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
         <v>106</v>
       </c>
@@ -9879,8 +9951,9 @@
       <c r="CH54" s="1"/>
       <c r="CI54" s="1"/>
       <c r="CJ54" s="1"/>
+      <c r="CK54" s="1"/>
     </row>
-    <row r="55" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
         <v>107</v>
       </c>
@@ -10079,8 +10152,9 @@
       <c r="CH55" s="1"/>
       <c r="CI55" s="1"/>
       <c r="CJ55" s="1"/>
+      <c r="CK55" s="1"/>
     </row>
-    <row r="56" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
         <v>95</v>
       </c>
@@ -10281,19 +10355,20 @@
       <c r="CH56" s="1"/>
       <c r="CI56" s="1"/>
       <c r="CJ56" s="1"/>
+      <c r="CK56" s="1"/>
     </row>
-    <row r="57" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
-        <v>96</v>
+        <v>232</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>31</v>
+        <v>233</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>158</v>
+        <v>234</v>
       </c>
       <c r="E57" s="2">
         <v>0</v>
@@ -10485,19 +10560,20 @@
       <c r="CH57" s="1"/>
       <c r="CI57" s="1"/>
       <c r="CJ57" s="1"/>
+      <c r="CK57" s="1"/>
     </row>
-    <row r="58" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A58" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E58" s="2">
         <v>0</v>
@@ -10691,19 +10767,20 @@
       <c r="CH58" s="1"/>
       <c r="CI58" s="1"/>
       <c r="CJ58" s="1"/>
+      <c r="CK58" s="1"/>
     </row>
-    <row r="59" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A59" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
@@ -10899,19 +10976,20 @@
       <c r="CH59" s="1"/>
       <c r="CI59" s="1"/>
       <c r="CJ59" s="1"/>
+      <c r="CK59" s="1"/>
     </row>
-    <row r="60" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A60" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D60" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E60" s="2">
         <v>0</v>
@@ -11109,19 +11187,20 @@
       <c r="CH60" s="1"/>
       <c r="CI60" s="1"/>
       <c r="CJ60" s="1"/>
+      <c r="CK60" s="1"/>
     </row>
-    <row r="61" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A61" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E61" s="2">
         <v>0</v>
@@ -11321,19 +11400,20 @@
       <c r="CH61" s="1"/>
       <c r="CI61" s="1"/>
       <c r="CJ61" s="1"/>
+      <c r="CK61" s="1"/>
     </row>
-    <row r="62" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E62" s="2">
         <v>0</v>
@@ -11535,19 +11615,20 @@
       <c r="CH62" s="1"/>
       <c r="CI62" s="1"/>
       <c r="CJ62" s="1"/>
+      <c r="CK62" s="1"/>
     </row>
-    <row r="63" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D63" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E63" s="2">
         <v>0</v>
@@ -11751,19 +11832,20 @@
       <c r="CH63" s="1"/>
       <c r="CI63" s="1"/>
       <c r="CJ63" s="1"/>
+      <c r="CK63" s="1"/>
     </row>
-    <row r="64" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E64" s="2">
         <v>0</v>
@@ -11969,19 +12051,20 @@
       <c r="CH64" s="1"/>
       <c r="CI64" s="1"/>
       <c r="CJ64" s="1"/>
+      <c r="CK64" s="1"/>
     </row>
-    <row r="65" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A65" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D65" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E65" s="2">
         <v>0</v>
@@ -12189,19 +12272,20 @@
       <c r="CH65" s="1"/>
       <c r="CI65" s="1"/>
       <c r="CJ65" s="1"/>
+      <c r="CK65" s="1"/>
     </row>
-    <row r="66" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A66" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E66" s="2">
         <v>0</v>
@@ -12411,46 +12495,47 @@
       <c r="CH66" s="1"/>
       <c r="CI66" s="1"/>
       <c r="CJ66" s="1"/>
+      <c r="CK66" s="1"/>
     </row>
-    <row r="67" spans="1:88" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D67" s="34" t="s">
-        <v>173</v>
+    <row r="67" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="A67" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" s="32" t="s">
+        <v>167</v>
       </c>
       <c r="E67" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F67" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G67" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J67" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K67" s="2">
         <v>1</v>
       </c>
-      <c r="L67" s="1">
-        <v>1</v>
+      <c r="L67" s="2">
+        <v>2</v>
       </c>
       <c r="M67" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N67" s="2">
         <v>0</v>
@@ -12462,124 +12547,124 @@
         <v>0</v>
       </c>
       <c r="Q67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB67" s="1">
         <v>1</v>
       </c>
       <c r="AC67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ67" s="1">
         <v>0</v>
       </c>
       <c r="AK67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA67" s="1">
         <v>0</v>
       </c>
       <c r="BB67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE67" s="1">
         <v>0</v>
@@ -12635,19 +12720,20 @@
       <c r="CH67" s="1"/>
       <c r="CI67" s="1"/>
       <c r="CJ67" s="1"/>
+      <c r="CK67" s="1"/>
     </row>
-    <row r="68" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="33" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E68" s="2">
         <v>2</v>
@@ -12659,16 +12745,16 @@
         <v>2</v>
       </c>
       <c r="H68" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I68" s="2">
         <v>2</v>
       </c>
       <c r="J68" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K68" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L68" s="1">
         <v>1</v>
@@ -12692,13 +12778,13 @@
         <v>1</v>
       </c>
       <c r="S68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V68" s="1">
         <v>1</v>
@@ -12710,16 +12796,16 @@
         <v>1</v>
       </c>
       <c r="Y68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC68" s="1">
         <v>1</v>
@@ -12743,7 +12829,7 @@
         <v>1</v>
       </c>
       <c r="AJ68" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK68" s="1">
         <v>1</v>
@@ -12803,7 +12889,7 @@
         <v>1</v>
       </c>
       <c r="BD68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE68" s="1">
         <v>0</v>
@@ -12836,7 +12922,7 @@
         <v>0</v>
       </c>
       <c r="BO68" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP68" s="1">
         <v>3</v>
@@ -12861,19 +12947,20 @@
       <c r="CH68" s="1"/>
       <c r="CI68" s="1"/>
       <c r="CJ68" s="1"/>
+      <c r="CK68" s="1"/>
     </row>
-    <row r="69" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D69" s="34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E69" s="2">
         <v>2</v>
@@ -12966,7 +13053,7 @@
         <v>1</v>
       </c>
       <c r="AI69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ69" s="1">
         <v>1</v>
@@ -13062,10 +13149,10 @@
         <v>0</v>
       </c>
       <c r="BO69" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ69" s="1">
         <v>3</v>
@@ -13089,19 +13176,20 @@
       <c r="CH69" s="1"/>
       <c r="CI69" s="1"/>
       <c r="CJ69" s="1"/>
+      <c r="CK69" s="1"/>
     </row>
-    <row r="70" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D70" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E70" s="2">
         <v>2</v>
@@ -13290,10 +13378,10 @@
         <v>0</v>
       </c>
       <c r="BO70" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP70" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ70" s="1">
         <v>0</v>
@@ -13319,19 +13407,20 @@
       <c r="CH70" s="1"/>
       <c r="CI70" s="1"/>
       <c r="CJ70" s="1"/>
+      <c r="CK70" s="1"/>
     </row>
-    <row r="71" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E71" s="2">
         <v>2</v>
@@ -13343,7 +13432,7 @@
         <v>2</v>
       </c>
       <c r="H71" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I71" s="2">
         <v>2</v>
@@ -13376,13 +13465,13 @@
         <v>1</v>
       </c>
       <c r="S71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V71" s="1">
         <v>1</v>
@@ -13394,13 +13483,13 @@
         <v>1</v>
       </c>
       <c r="Y71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB71" s="1">
         <v>0</v>
@@ -13427,13 +13516,13 @@
         <v>0</v>
       </c>
       <c r="AJ71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM71" s="1">
         <v>1</v>
@@ -13448,34 +13537,34 @@
         <v>1</v>
       </c>
       <c r="AQ71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS71" s="1">
         <v>1</v>
       </c>
       <c r="AT71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA71" s="1">
         <v>0</v>
@@ -13484,7 +13573,7 @@
         <v>1</v>
       </c>
       <c r="BC71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD71" s="1">
         <v>0</v>
@@ -13520,16 +13609,16 @@
         <v>0</v>
       </c>
       <c r="BO71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP71" s="1">
         <v>1</v>
       </c>
       <c r="BQ71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS71" s="1">
         <v>3</v>
@@ -13551,43 +13640,44 @@
       <c r="CH71" s="1"/>
       <c r="CI71" s="1"/>
       <c r="CJ71" s="1"/>
+      <c r="CK71" s="1"/>
     </row>
-    <row r="72" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D72" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E72" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F72" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G72" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H72" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J72" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K72" s="2">
         <v>0</v>
       </c>
       <c r="L72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M72" s="2">
         <v>0</v>
@@ -13605,55 +13695,55 @@
         <v>0</v>
       </c>
       <c r="R72" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI72" s="1">
         <v>0</v>
@@ -13668,16 +13758,16 @@
         <v>0</v>
       </c>
       <c r="AM72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ72" s="1">
         <v>0</v>
@@ -13686,7 +13776,7 @@
         <v>0</v>
       </c>
       <c r="AS72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT72" s="1">
         <v>0</v>
@@ -13710,7 +13800,7 @@
         <v>0</v>
       </c>
       <c r="BA72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB72" s="1">
         <v>1</v>
@@ -13755,16 +13845,16 @@
         <v>0</v>
       </c>
       <c r="BP72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT72" s="1">
         <v>3</v>
@@ -13785,37 +13875,38 @@
       <c r="CH72" s="1"/>
       <c r="CI72" s="1"/>
       <c r="CJ72" s="1"/>
+      <c r="CK72" s="1"/>
     </row>
-    <row r="73" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D73" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E73" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F73" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G73" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H73" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I73" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J73" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K73" s="2">
         <v>0</v>
@@ -13842,34 +13933,34 @@
         <v>0</v>
       </c>
       <c r="S73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC73" s="1">
         <v>0</v>
@@ -13944,7 +14035,7 @@
         <v>0</v>
       </c>
       <c r="BA73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB73" s="1">
         <v>1</v>
@@ -14021,40 +14112,41 @@
       <c r="CH73" s="1"/>
       <c r="CI73" s="1"/>
       <c r="CJ73" s="1"/>
+      <c r="CK73" s="1"/>
     </row>
-    <row r="74" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D74" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E74" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F74" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G74" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J74" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K74" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L74" s="1">
         <v>0</v>
@@ -14063,7 +14155,7 @@
         <v>0</v>
       </c>
       <c r="N74" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O74" s="2">
         <v>0</v>
@@ -14078,34 +14170,34 @@
         <v>0</v>
       </c>
       <c r="S74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC74" s="1">
         <v>0</v>
@@ -14259,19 +14351,20 @@
       <c r="CH74" s="1"/>
       <c r="CI74" s="1"/>
       <c r="CJ74" s="1"/>
+      <c r="CK74" s="1"/>
     </row>
-    <row r="75" spans="1:88" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D75" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E75" s="2">
         <v>0</v>
@@ -14499,19 +14592,20 @@
       <c r="CH75" s="1"/>
       <c r="CI75" s="1"/>
       <c r="CJ75" s="1"/>
+      <c r="CK75" s="1"/>
     </row>
-    <row r="76" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:89" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D76" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E76" s="2">
         <v>0</v>
@@ -14541,16 +14635,16 @@
         <v>0</v>
       </c>
       <c r="N76" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O76" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P76" s="2">
         <v>0</v>
       </c>
       <c r="Q76" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R76" s="2">
         <v>0</v>
@@ -14658,13 +14752,13 @@
         <v>0</v>
       </c>
       <c r="BA76" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB76" s="1">
         <v>1</v>
       </c>
       <c r="BC76" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD76" s="1">
         <v>0</v>
@@ -14741,19 +14835,20 @@
       <c r="CH76" s="1"/>
       <c r="CI76" s="1"/>
       <c r="CJ76" s="1"/>
+      <c r="CK76" s="1"/>
     </row>
-    <row r="77" spans="1:88" ht="60" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D77" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E77" s="2">
         <v>0</v>
@@ -14985,19 +15080,20 @@
       <c r="CH77" s="1"/>
       <c r="CI77" s="1"/>
       <c r="CJ77" s="1"/>
+      <c r="CK77" s="1"/>
     </row>
-    <row r="78" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:89" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D78" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E78" s="2">
         <v>0</v>
@@ -15018,7 +15114,7 @@
         <v>2</v>
       </c>
       <c r="K78" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L78" s="1">
         <v>0</v>
@@ -15030,13 +15126,13 @@
         <v>0</v>
       </c>
       <c r="O78" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P78" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q78" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R78" s="2">
         <v>0</v>
@@ -15144,13 +15240,13 @@
         <v>0</v>
       </c>
       <c r="BA78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB78" s="1">
         <v>1</v>
       </c>
       <c r="BC78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD78" s="1">
         <v>0</v>
@@ -15231,19 +15327,20 @@
       <c r="CH78" s="1"/>
       <c r="CI78" s="1"/>
       <c r="CJ78" s="1"/>
+      <c r="CK78" s="1"/>
     </row>
-    <row r="79" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D79" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E79" s="2">
         <v>0</v>
@@ -15479,19 +15576,20 @@
       <c r="CH79" s="1"/>
       <c r="CI79" s="1"/>
       <c r="CJ79" s="1"/>
+      <c r="CK79" s="1"/>
     </row>
-    <row r="80" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D80" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E80" s="2">
         <v>0</v>
@@ -15729,19 +15827,20 @@
       <c r="CH80" s="1"/>
       <c r="CI80" s="1"/>
       <c r="CJ80" s="1"/>
+      <c r="CK80" s="1"/>
     </row>
-    <row r="81" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D81" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E81" s="2">
         <v>0</v>
@@ -15981,19 +16080,20 @@
       <c r="CH81" s="1"/>
       <c r="CI81" s="1"/>
       <c r="CJ81" s="1"/>
+      <c r="CK81" s="1"/>
     </row>
-    <row r="82" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D82" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E82" s="2">
         <v>0</v>
@@ -16235,19 +16335,20 @@
       <c r="CH82" s="1"/>
       <c r="CI82" s="1"/>
       <c r="CJ82" s="1"/>
+      <c r="CK82" s="1"/>
     </row>
-    <row r="83" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="33" t="s">
-        <v>225</v>
+        <v>123</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>224</v>
+        <v>58</v>
       </c>
       <c r="D83" s="34" t="s">
-        <v>226</v>
+        <v>185</v>
       </c>
       <c r="E83" s="2">
         <v>0</v>
@@ -16268,7 +16369,7 @@
         <v>2</v>
       </c>
       <c r="K83" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L83" s="1">
         <v>0</v>
@@ -16283,10 +16384,10 @@
         <v>0</v>
       </c>
       <c r="P83" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q83" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R83" s="2">
         <v>0</v>
@@ -16394,49 +16495,49 @@
         <v>0</v>
       </c>
       <c r="BA83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB83" s="1">
         <v>1</v>
       </c>
       <c r="BC83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP83" s="1">
         <v>0</v>
@@ -16451,7 +16552,7 @@
         <v>0</v>
       </c>
       <c r="BT83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU83" s="1">
         <v>0</v>
@@ -16469,19 +16570,19 @@
         <v>0</v>
       </c>
       <c r="BZ83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE83" s="1">
         <v>3</v>
@@ -16491,19 +16592,20 @@
       <c r="CH83" s="1"/>
       <c r="CI83" s="1"/>
       <c r="CJ83" s="1"/>
+      <c r="CK83" s="1"/>
     </row>
-    <row r="84" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="33" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D84" s="34" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E84" s="2">
         <v>0</v>
@@ -16662,7 +16764,7 @@
         <v>1</v>
       </c>
       <c r="BE84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF84" s="1">
         <v>1</v>
@@ -16695,7 +16797,7 @@
         <v>1</v>
       </c>
       <c r="BP84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ84" s="1">
         <v>0</v>
@@ -16707,10 +16809,10 @@
         <v>0</v>
       </c>
       <c r="BT84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV84" s="1">
         <v>0</v>
@@ -16725,7 +16827,7 @@
         <v>0</v>
       </c>
       <c r="BZ84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA84" s="1">
         <v>1</v>
@@ -16740,7 +16842,7 @@
         <v>1</v>
       </c>
       <c r="CE84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF84" s="1">
         <v>3</v>
@@ -16749,19 +16851,20 @@
       <c r="CH84" s="1"/>
       <c r="CI84" s="1"/>
       <c r="CJ84" s="1"/>
+      <c r="CK84" s="1"/>
     </row>
-    <row r="85" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="33" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D85" s="34" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="E85" s="2">
         <v>0</v>
@@ -16953,7 +17056,7 @@
         <v>1</v>
       </c>
       <c r="BP85" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ85" s="1">
         <v>0</v>
@@ -16965,10 +17068,10 @@
         <v>0</v>
       </c>
       <c r="BT85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU85" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV85" s="1">
         <v>0</v>
@@ -16983,7 +17086,7 @@
         <v>0</v>
       </c>
       <c r="BZ85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA85" s="1">
         <v>1</v>
@@ -16998,7 +17101,7 @@
         <v>1</v>
       </c>
       <c r="CE85" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF85" s="1">
         <v>0</v>
@@ -17009,19 +17112,20 @@
       <c r="CH85" s="1"/>
       <c r="CI85" s="1"/>
       <c r="CJ85" s="1"/>
+      <c r="CK85" s="1"/>
     </row>
-    <row r="86" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A86" s="33" t="s">
-        <v>124</v>
+        <v>227</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="D86" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E86" s="2">
         <v>0</v>
@@ -17168,7 +17272,7 @@
         <v>0</v>
       </c>
       <c r="BA86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB86" s="1">
         <v>1</v>
@@ -17177,43 +17281,43 @@
         <v>1</v>
       </c>
       <c r="BD86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ86" s="1">
         <v>0</v>
@@ -17228,7 +17332,7 @@
         <v>0</v>
       </c>
       <c r="BU86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV86" s="1">
         <v>0</v>
@@ -17246,19 +17350,19 @@
         <v>0</v>
       </c>
       <c r="CA86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF86" s="1">
         <v>0</v>
@@ -17271,40 +17375,41 @@
       </c>
       <c r="CI86" s="1"/>
       <c r="CJ86" s="1"/>
+      <c r="CK86" s="1"/>
     </row>
-    <row r="87" spans="1:88" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:89" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D87" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E87" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F87" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G87" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H87" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I87" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J87" s="2">
         <v>2</v>
       </c>
       <c r="K87" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L87" s="1">
         <v>0</v>
@@ -17328,31 +17433,31 @@
         <v>0</v>
       </c>
       <c r="S87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB87" s="1">
         <v>1</v>
@@ -17475,13 +17580,13 @@
         <v>0</v>
       </c>
       <c r="BP87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS87" s="1">
         <v>0</v>
@@ -17499,7 +17604,7 @@
         <v>0</v>
       </c>
       <c r="BX87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY87" s="1">
         <v>0</v>
@@ -17523,10 +17628,10 @@
         <v>0</v>
       </c>
       <c r="CF87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH87" s="1">
         <v>0</v>
@@ -17535,19 +17640,20 @@
         <v>3</v>
       </c>
       <c r="CJ87" s="1"/>
+      <c r="CK87" s="1"/>
     </row>
-    <row r="88" spans="1:88" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="B88" s="36" t="s">
+    <row r="88" spans="1:89" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C88" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="D88" s="37" t="s">
-        <v>189</v>
+      <c r="C88" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D88" s="34" t="s">
+        <v>188</v>
       </c>
       <c r="E88" s="2">
         <v>2</v>
@@ -17565,10 +17671,10 @@
         <v>2</v>
       </c>
       <c r="J88" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K88" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L88" s="1">
         <v>0</v>
@@ -17586,7 +17692,7 @@
         <v>0</v>
       </c>
       <c r="Q88" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R88" s="2">
         <v>0</v>
@@ -17619,7 +17725,7 @@
         <v>1</v>
       </c>
       <c r="AB88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC88" s="1">
         <v>0</v>
@@ -17634,10 +17740,10 @@
         <v>0</v>
       </c>
       <c r="AG88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI88" s="1">
         <v>0</v>
@@ -17697,10 +17803,10 @@
         <v>0</v>
       </c>
       <c r="BB88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD88" s="1">
         <v>0</v>
@@ -17736,19 +17842,19 @@
         <v>0</v>
       </c>
       <c r="BO88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT88" s="1">
         <v>0</v>
@@ -17766,7 +17872,7 @@
         <v>0</v>
       </c>
       <c r="BY88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ88" s="1">
         <v>0</v>
@@ -17790,10 +17896,10 @@
         <v>0</v>
       </c>
       <c r="CG88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI88" s="1">
         <v>0</v>
@@ -17801,10 +17907,280 @@
       <c r="CJ88" s="1">
         <v>3</v>
       </c>
+      <c r="CK88" s="1"/>
+    </row>
+    <row r="89" spans="1:89" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B89" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C89" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D89" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="E89" s="2">
+        <v>2</v>
+      </c>
+      <c r="F89" s="2">
+        <v>2</v>
+      </c>
+      <c r="G89" s="2">
+        <v>2</v>
+      </c>
+      <c r="H89" s="2">
+        <v>1</v>
+      </c>
+      <c r="I89" s="2">
+        <v>2</v>
+      </c>
+      <c r="J89" s="2">
+        <v>0</v>
+      </c>
+      <c r="K89" s="2">
+        <v>0</v>
+      </c>
+      <c r="L89" s="1">
+        <v>0</v>
+      </c>
+      <c r="M89" s="2">
+        <v>0</v>
+      </c>
+      <c r="N89" s="2">
+        <v>0</v>
+      </c>
+      <c r="O89" s="2">
+        <v>0</v>
+      </c>
+      <c r="P89" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q89" s="2">
+        <v>0</v>
+      </c>
+      <c r="R89" s="2">
+        <v>0</v>
+      </c>
+      <c r="S89" s="1">
+        <v>1</v>
+      </c>
+      <c r="T89" s="1">
+        <v>1</v>
+      </c>
+      <c r="U89" s="1">
+        <v>1</v>
+      </c>
+      <c r="V89" s="1">
+        <v>1</v>
+      </c>
+      <c r="W89" s="1">
+        <v>1</v>
+      </c>
+      <c r="X89" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y89" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH89" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY89" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP89" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ89" s="1">
+        <v>1</v>
+      </c>
+      <c r="BR89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BS89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BT89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BU89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY89" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ89" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK89" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:CJ4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A1:CJ88">
+  <autoFilter ref="A4:CK4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A1:CK89">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
bugfixes - qlang sort instruction applied changes inplace - deduplicate used verbosity=0 as default
Changes to be committed:
	modified:   qplib/data/symbols.csv
	modified:   qplib/data/symbols.xlsx
	modified:   qplib/pandas.py
	modified:   qplib/qlang.py
</commit_message>
<xml_diff>
--- a/qplib/data/symbols.xlsx
+++ b/qplib/data/symbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MartinVölkl\Desktop\qplib_dev\qplib\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E60AF1-135C-4706-A1AD-C5801E9FF9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84E5E45-67B9-40D0-A1EA-5BD7BADEEA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1491,7 +1491,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="P55" sqref="P55"/>
+      <selection pane="bottomRight" activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10204,7 +10204,7 @@
         <v>0</v>
       </c>
       <c r="Q56" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R56" s="2">
         <v>0</v>

</xml_diff>